<commit_message>
Changed the notebook for plotting BFS normalized times and other charts with new datapoints
</commit_message>
<xml_diff>
--- a/outputs/LazyPLots.xlsx
+++ b/outputs/LazyPLots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Puneet89/scratch/margraphita/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC094529-9768-1C4F-858C-FFF93FA1B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC7D87-F63A-CC41-A13F-75E9BC5C5F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="9" xr2:uid="{F5B2087C-EB84-EA45-874C-018D03B7F2D7}"/>
   </bookViews>
@@ -27,24 +27,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Bulk insert'!$A$3:$G$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sheet1!$A$1:$T$97</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'fixed bulk times'!$AA$47</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'fixed bulk times'!$AA$48:$AA$65</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'fixed bulk times'!$AB$47</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'fixed bulk times'!$AB$48:$AB$65</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'fixed bulk times'!$AC$47</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'fixed bulk times'!$AC$48:$AC$65</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'fixed bulk times'!$Y$48:$Y$65</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'fixed bulk times'!$Z$47</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'fixed bulk times'!$Z$48:$Z$65</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">'fixed bulk times'!$AA$48:$AA$65</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">'fixed bulk times'!$AB$47</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">'fixed bulk times'!$AB$48:$AB$65</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">'fixed bulk times'!$AC$47</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">'fixed bulk times'!$AC$48:$AC$65</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">'fixed bulk times'!$Y$48:$Y$65</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">'fixed bulk times'!$Z$47</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">'fixed bulk times'!$Z$48:$Z$65</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">'fixed bulk times'!$AA$47</definedName>
     <definedName name="adj_kron_insert_times" localSheetId="2">'Bulk insert'!$A$21:$E$36</definedName>
     <definedName name="adj_rd_cit_Patents_bfs" localSheetId="5">BFS!$B$2:$G$66</definedName>
     <definedName name="adj_rd_cit_Patents_pr" localSheetId="3">PR!$B$2:$N$27</definedName>
@@ -1935,7 +1917,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1945,6 +1927,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2066,7 +2054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2155,9 +2143,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2190,6 +2175,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2224,6 +2212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -6760,51 +6749,51 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="std_kron_insert_times" connectionId="40" xr16:uid="{DD58A6D3-3D02-1744-81FD-D588AE2BB621}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="insert_1" connectionId="29" xr16:uid="{33E24452-5EC7-E640-807C-88562445B378}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s17_e8_pr" connectionId="26" xr16:uid="{A90E1AB3-33BE-0847-AE98-484E06AA50DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s14_e8_pr" connectionId="10" xr16:uid="{A44DD4B7-3783-C74C-90A9-F5300ED43C91}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s16_e8_pr" connectionId="25" xr16:uid="{0AC7AA9F-F6B2-BA43-8410-2370AEBAABF2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s14_e8_pr" connectionId="23" xr16:uid="{B4171653-78A5-F84E-8D26-DAC4BE62C1EB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s13_e8_pr_1" connectionId="9" xr16:uid="{AEC14F0D-DFAE-934E-8A3E-4482DC241F7D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_cit-Patents_pr" connectionId="3" xr16:uid="{485EE36F-FDDB-994D-966D-522E9628BB05}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s11_e8_pr" connectionId="21" xr16:uid="{8E9AD936-CDDC-F446-BEBB-6CD7FE815D55}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s12_e8_pr" connectionId="22" xr16:uid="{C05B0550-64F8-5345-8294-543CC69692C2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s19_e8_pr" connectionId="15" xr16:uid="{9C3F3370-E7FF-0E40-9B03-919C89070B0B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s15_e8_pr" connectionId="24" xr16:uid="{37C6A0ED-93B0-4E47-A0CC-DD5C864B8623}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s12_e8_pr" connectionId="7" xr16:uid="{3D563C20-93B9-6543-A779-8AE817951D58}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s18_e8_pr_1" connectionId="27" xr16:uid="{86B50108-FE89-8446-86C2-A84FEB9436A7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s11_e8_pr" connectionId="21" xr16:uid="{8E9AD936-CDDC-F446-BEBB-6CD7FE815D55}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s10_e8_pr" connectionId="20" xr16:uid="{6C29FD2B-EA3F-8D4B-AAFB-F9BC7FFE4E49}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s13_e8_pr" connectionId="8" xr16:uid="{DAF29A3E-0401-1D42-BD6D-97CECD422B68}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s16_e8_pr" connectionId="12" xr16:uid="{A722C098-BD83-EF49-8157-E9EB379A71BB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s19_e8_pr" connectionId="28" xr16:uid="{B3509AB6-E6E6-1449-B7FE-D5D0DEE861A2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_cit-Patents_pr" connectionId="3" xr16:uid="{485EE36F-FDDB-994D-966D-522E9628BB05}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_cit-Patents_pr" connectionId="18" xr16:uid="{5F7237CE-B0C6-DA4C-8854-AF51F9C6D01C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="insert_1" connectionId="29" xr16:uid="{33E24452-5EC7-E640-807C-88562445B378}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_kron_insert_times" connectionId="16" xr16:uid="{342679E8-4467-A941-85AF-CFDDC1E9026C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6812,23 +6801,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s10_e8_pr" connectionId="20" xr16:uid="{6C29FD2B-EA3F-8D4B-AAFB-F9BC7FFE4E49}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s15_e8_pr" connectionId="11" xr16:uid="{95FB7F31-C318-C345-A4C9-BFCD1FF00EC3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s10_e8_pr" connectionId="5" xr16:uid="{AFCFFA7D-279B-2142-905B-3BFEF65649F8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="std_rd_cit-Patents_pr" connectionId="42" xr16:uid="{8A184221-111F-FC49-B436-A1A0B44AE26B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s16_e8_pr" connectionId="25" xr16:uid="{0AC7AA9F-F6B2-BA43-8410-2370AEBAABF2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s13_e8_pr_1" connectionId="9" xr16:uid="{AEC14F0D-DFAE-934E-8A3E-4482DC241F7D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s13_e8_pr" connectionId="8" xr16:uid="{DAF29A3E-0401-1D42-BD6D-97CECD422B68}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_cit-Patents_pr" connectionId="18" xr16:uid="{5F7237CE-B0C6-DA4C-8854-AF51F9C6D01C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s15_e8_pr" connectionId="24" xr16:uid="{37C6A0ED-93B0-4E47-A0CC-DD5C864B8623}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6836,15 +6825,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s14_e8_pr" connectionId="10" xr16:uid="{A44DD4B7-3783-C74C-90A9-F5300ED43C91}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s16_e8_pr" connectionId="12" xr16:uid="{A722C098-BD83-EF49-8157-E9EB379A71BB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s12_e8_pr" connectionId="22" xr16:uid="{C05B0550-64F8-5345-8294-543CC69692C2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s18_e8_pr" connectionId="14" xr16:uid="{731EF252-DB53-8244-97FB-8D5CC6DAB673}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s15_e8_pr" connectionId="11" xr16:uid="{95FB7F31-C318-C345-A4C9-BFCD1FF00EC3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="std_rd_cit-Patents_pr" connectionId="42" xr16:uid="{8A184221-111F-FC49-B436-A1A0B44AE26B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6852,43 +6841,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s18_e8_pr" connectionId="14" xr16:uid="{731EF252-DB53-8244-97FB-8D5CC6DAB673}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s12_e8_pr" connectionId="7" xr16:uid="{3D563C20-93B9-6543-A779-8AE817951D58}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_cit-Patents_bfs" connectionId="2" xr16:uid="{068D0F8D-84CB-1944-916B-E99DA667AB5A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s10_e8_bfs" connectionId="19" xr16:uid="{9BB78720-03CE-D745-B3B0-89F5C53100E2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_s10_e8_bfs" connectionId="4" xr16:uid="{3A280166-0A7E-3648-8193-A80D6A717037}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="std_rd_cit-Patents_bfs" connectionId="41" xr16:uid="{94102776-A9DA-E342-8240-AE2D28BFD550}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_cit-Patents_bfs" connectionId="17" xr16:uid="{A5507376-E57D-DA48-A6D4-5C93BD5FCB12}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="adj_rd_cit-Patents_bfs" connectionId="2" xr16:uid="{068D0F8D-84CB-1944-916B-E99DA667AB5A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="python_insert" connectionId="35" xr16:uid="{AA9AAA56-2FA9-9F4E-B7D8-47A38E88ECEF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="merged_kron_insert_1" connectionId="32" xr16:uid="{79C33162-66EE-1A4B-A93A-56069E48A775}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="merged_kron_insert_1" connectionId="32" xr16:uid="{79C33162-66EE-1A4B-A93A-56069E48A775}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="single_threaded_kron_inserts_cpp_1" connectionId="37" xr16:uid="{7A7E832D-BDE0-9B4D-8532-FADE7DC5A767}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="single_threaded_kron_inserts_cpp_1" connectionId="37" xr16:uid="{7A7E832D-BDE0-9B4D-8532-FADE7DC5A767}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="single_threaded_kron_inserts_cpp" connectionId="36" xr16:uid="{6D3F7C47-EE2D-B049-ADC9-AF6792A45A68}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="single_threaded_kron_inserts_cpp" connectionId="36" xr16:uid="{6D3F7C47-EE2D-B049-ADC9-AF6792A45A68}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="python_insert" connectionId="35" xr16:uid="{AA9AAA56-2FA9-9F4E-B7D8-47A38E88ECEF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6916,15 +6905,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_kron_insert_times" connectionId="16" xr16:uid="{342679E8-4467-A941-85AF-CFDDC1E9026C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="std_kron_insert_times" connectionId="40" xr16:uid="{DD58A6D3-3D02-1744-81FD-D588AE2BB621}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s17_e8_pr" connectionId="26" xr16:uid="{A90E1AB3-33BE-0847-AE98-484E06AA50DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s19_e8_pr" connectionId="28" xr16:uid="{B3509AB6-E6E6-1449-B7FE-D5D0DEE861A2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s14_e8_pr" connectionId="23" xr16:uid="{B4171653-78A5-F84E-8D26-DAC4BE62C1EB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ekey_rd_s18_e8_pr_1" connectionId="27" xr16:uid="{86B50108-FE89-8446-86C2-A84FEB9436A7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8153,12 +8142,12 @@
       <c r="Y37" s="2"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="E38" s="38" t="s">
+      <c r="E38" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
       <c r="I38" s="6" t="s">
         <v>307</v>
       </c>
@@ -8528,8 +8517,8 @@
       <c r="T49" s="6"/>
     </row>
     <row r="54" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AN54" s="39"/>
-      <c r="AO54" s="40"/>
+      <c r="AN54" s="38"/>
+      <c r="AO54" s="39"/>
       <c r="AP54" s="37" t="s">
         <v>314</v>
       </c>
@@ -8692,11 +8681,11 @@
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="41" t="s">
+      <c r="H59" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="41"/>
       <c r="U59" t="s">
         <v>173</v>
       </c>
@@ -9196,11 +9185,11 @@
       <c r="W65">
         <v>1810259</v>
       </c>
-      <c r="AK65" s="43" t="s">
+      <c r="AK65" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="AL65" s="44"/>
-      <c r="AM65" s="45"/>
+      <c r="AL65" s="43"/>
+      <c r="AM65" s="44"/>
       <c r="AN65" s="11">
         <f>ROUNDUP(AVERAGE(AQ56:AQ64),0)</f>
         <v>644393</v>
@@ -9976,16 +9965,16 @@
     </row>
     <row r="92" spans="5:22" x14ac:dyDescent="0.2">
       <c r="F92" s="8"/>
-      <c r="G92" s="46" t="s">
+      <c r="G92" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="H92" s="46"/>
+      <c r="H92" s="45"/>
       <c r="I92" s="8"/>
-      <c r="J92" s="47" t="s">
+      <c r="J92" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="K92" s="48"/>
-      <c r="L92" s="49"/>
+      <c r="K92" s="47"/>
+      <c r="L92" s="48"/>
       <c r="M92" s="21" t="s">
         <v>226</v>
       </c>
@@ -12228,6 +12217,11 @@
     <sortCondition ref="F94:F102"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="J120:L120"/>
     <mergeCell ref="AR54:AS54"/>
     <mergeCell ref="AT54:AU54"/>
     <mergeCell ref="AN54:AO54"/>
@@ -12237,11 +12231,6 @@
     <mergeCell ref="G92:H92"/>
     <mergeCell ref="J92:L92"/>
     <mergeCell ref="AP54:AQ54"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="J120:L120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45212,27 +45201,27 @@
       </c>
     </row>
     <row r="104" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B104" s="42" t="s">
+      <c r="B104" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="C104" s="42"/>
-      <c r="D104" s="42"/>
-      <c r="E104" s="42"/>
-      <c r="F104" s="42"/>
-      <c r="G104" s="42" t="s">
+      <c r="C104" s="41"/>
+      <c r="D104" s="41"/>
+      <c r="E104" s="41"/>
+      <c r="F104" s="41"/>
+      <c r="G104" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="H104" s="42"/>
-      <c r="I104" s="42"/>
-      <c r="J104" s="42"/>
-      <c r="K104" s="42"/>
-      <c r="L104" s="42"/>
-      <c r="N104" s="42"/>
-      <c r="O104" s="42"/>
-      <c r="P104" s="42"/>
-      <c r="Q104" s="42"/>
-      <c r="R104" s="42"/>
-      <c r="S104" s="42"/>
+      <c r="H104" s="41"/>
+      <c r="I104" s="41"/>
+      <c r="J104" s="41"/>
+      <c r="K104" s="41"/>
+      <c r="L104" s="41"/>
+      <c r="N104" s="41"/>
+      <c r="O104" s="41"/>
+      <c r="P104" s="41"/>
+      <c r="Q104" s="41"/>
+      <c r="R104" s="41"/>
+      <c r="S104" s="41"/>
       <c r="V104" t="s">
         <v>173</v>
       </c>
@@ -47724,8 +47713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F324DA-6DBC-1A4F-9AFD-28C98EDAF4DF}">
   <dimension ref="A1:AE87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T19" workbookViewId="0">
-      <selection activeCell="AC48" sqref="AC48:AC65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="T77" sqref="T77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47824,76 +47813,76 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D3">
-        <v>854</v>
+        <v>1628</v>
       </c>
       <c r="E3">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="F3">
-        <v>36768</v>
+        <v>66558</v>
       </c>
       <c r="G3">
-        <v>20012</v>
+        <v>40174</v>
       </c>
       <c r="H3">
-        <v>4182</v>
+        <v>8415</v>
       </c>
       <c r="I3">
-        <v>2463</v>
+        <v>19460</v>
       </c>
       <c r="J3">
         <f>SUM(F3:I3)/10</f>
-        <v>6342.5</v>
+        <v>13460.7</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K44" si="0">J3*0.000001</f>
-        <v>6.3425E-3</v>
+        <f>J3*0.000001</f>
+        <v>1.3460700000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>323</v>
+        <v>162</v>
+      </c>
+      <c r="C4" t="s">
+        <v>325</v>
       </c>
       <c r="D4">
-        <v>854</v>
+        <v>3115</v>
       </c>
       <c r="E4">
-        <v>8192</v>
-      </c>
-      <c r="F4" s="31">
-        <v>35106</v>
+        <v>32768</v>
+      </c>
+      <c r="F4">
+        <v>138235</v>
       </c>
       <c r="G4">
-        <v>18933</v>
+        <v>113681</v>
       </c>
       <c r="H4">
-        <v>4157</v>
+        <v>8403</v>
       </c>
       <c r="I4">
-        <v>2165</v>
+        <v>38353</v>
       </c>
       <c r="J4">
         <f>SUM(F4:I4)/10</f>
-        <v>6036.1</v>
+        <v>29867.200000000001</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>6.0361E-3</v>
+        <f>J4*0.000001</f>
+        <v>2.98672E-2</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -47901,110 +47890,110 @@
         <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D5">
-        <v>1628</v>
+        <v>5990</v>
       </c>
       <c r="E5">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="F5">
-        <v>66558</v>
+        <v>262462</v>
       </c>
       <c r="G5">
-        <v>40174</v>
+        <v>190518</v>
       </c>
       <c r="H5">
-        <v>8415</v>
+        <v>35064</v>
       </c>
       <c r="I5">
-        <v>19460</v>
+        <v>75107</v>
       </c>
       <c r="J5">
         <f>SUM(F5:I5)/10</f>
-        <v>13460.7</v>
+        <v>56315.1</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>1.3460700000000001E-2</v>
+        <f>J5*0.000001</f>
+        <v>5.6315099999999993E-2</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D6">
-        <v>1628</v>
+        <v>11545</v>
       </c>
       <c r="E6">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="F6">
-        <v>68258</v>
+        <v>538286</v>
       </c>
       <c r="G6">
-        <v>40767</v>
+        <v>343296</v>
       </c>
       <c r="H6">
-        <v>9274</v>
+        <v>79318</v>
       </c>
       <c r="I6">
-        <v>5131</v>
+        <v>160466</v>
       </c>
       <c r="J6">
         <f>SUM(F6:I6)/10</f>
-        <v>12343</v>
+        <v>112136.6</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1.2343E-2</v>
+        <f>J6*0.000001</f>
+        <v>0.1121366</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D7">
-        <v>1628</v>
+        <v>22128</v>
       </c>
       <c r="E7">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="F7">
-        <v>67869</v>
+        <v>1157352</v>
       </c>
       <c r="G7">
-        <v>39739</v>
+        <v>725762</v>
       </c>
       <c r="H7">
-        <v>9486</v>
+        <v>156026</v>
       </c>
       <c r="I7">
-        <v>3698</v>
+        <v>373368</v>
       </c>
       <c r="J7">
         <f>SUM(F7:I7)/10</f>
-        <v>12079.2</v>
+        <v>241250.8</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>1.20792E-2</v>
+        <f>J7*0.000001</f>
+        <v>0.24125079999999999</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -48012,110 +48001,110 @@
         <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D8">
-        <v>3115</v>
+        <v>42369</v>
       </c>
       <c r="E8">
-        <v>32768</v>
+        <v>524288</v>
       </c>
       <c r="F8">
-        <v>138235</v>
+        <v>2289625</v>
       </c>
       <c r="G8">
-        <v>113681</v>
+        <v>1406313</v>
       </c>
       <c r="H8">
-        <v>8403</v>
+        <v>318242</v>
       </c>
       <c r="I8">
-        <v>38353</v>
+        <v>1011954</v>
       </c>
       <c r="J8">
         <f>SUM(F8:I8)/10</f>
-        <v>29867.200000000001</v>
+        <v>502613.4</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>2.98672E-2</v>
+        <f>J8*0.000001</f>
+        <v>0.50261339999999999</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="D9">
-        <v>3115</v>
+        <v>81468</v>
       </c>
       <c r="E9">
-        <v>32768</v>
+        <v>1048576</v>
       </c>
       <c r="F9">
-        <v>133543</v>
+        <v>4720035</v>
       </c>
       <c r="G9">
-        <v>89269</v>
+        <v>2942968</v>
       </c>
       <c r="H9">
-        <v>18697</v>
+        <v>600752</v>
       </c>
       <c r="I9">
-        <v>8792</v>
+        <v>1381023</v>
       </c>
       <c r="J9">
         <f>SUM(F9:I9)/10</f>
-        <v>25030.1</v>
+        <v>964477.8</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>2.5030099999999996E-2</v>
+        <f>J9*0.000001</f>
+        <v>0.96447780000000005</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="D10">
-        <v>3115</v>
+        <v>155576</v>
       </c>
       <c r="E10">
-        <v>32768</v>
+        <v>2097152</v>
       </c>
       <c r="F10">
-        <v>132636</v>
+        <v>10869235</v>
       </c>
       <c r="G10">
-        <v>103646</v>
+        <v>5625590</v>
       </c>
       <c r="H10">
-        <v>17914</v>
+        <v>1192874</v>
       </c>
       <c r="I10">
-        <v>6273</v>
+        <v>2779336</v>
       </c>
       <c r="J10">
         <f>SUM(F10:I10)/10</f>
-        <v>26046.9</v>
+        <v>2046703.5</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>2.6046900000000001E-2</v>
+        <f>J10*0.000001</f>
+        <v>2.0467035</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="37" t="s">
@@ -48134,36 +48123,36 @@
         <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="D11">
-        <v>5990</v>
+        <v>296688</v>
       </c>
       <c r="E11">
-        <v>65536</v>
+        <v>4194304</v>
       </c>
       <c r="F11">
-        <v>262462</v>
+        <v>22938768</v>
       </c>
       <c r="G11">
-        <v>190518</v>
+        <v>12492948</v>
       </c>
       <c r="H11">
-        <v>35064</v>
+        <v>2289086</v>
       </c>
       <c r="I11">
-        <v>75107</v>
+        <v>5626806</v>
       </c>
       <c r="J11">
         <f>SUM(F11:I11)/10</f>
-        <v>56315.1</v>
+        <v>4334760.8</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>5.6315099999999993E-2</v>
+        <f>J11*0.000001</f>
+        <v>4.3347607999999997</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>154</v>
@@ -48198,39 +48187,39 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D12">
-        <v>5990</v>
+        <v>575281</v>
       </c>
       <c r="E12">
-        <v>65536</v>
+        <v>8388608</v>
       </c>
       <c r="F12">
-        <v>262083</v>
+        <v>51632958</v>
       </c>
       <c r="G12">
-        <v>158521</v>
+        <v>24887442</v>
       </c>
       <c r="H12">
-        <v>36176</v>
+        <v>4527503</v>
       </c>
       <c r="I12">
-        <v>17855</v>
+        <v>12745590</v>
       </c>
       <c r="J12">
         <f>SUM(F12:I12)/10</f>
-        <v>47463.5</v>
+        <v>9379349.3000000007</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>4.7463499999999999E-2</v>
+        <f>J12*0.000001</f>
+        <v>9.3793492999999994</v>
       </c>
       <c r="L12" t="s">
         <v>160</v>
@@ -48245,65 +48234,65 @@
         <v>0.62609696388244596</v>
       </c>
       <c r="P12">
-        <f t="shared" ref="P12:P22" si="1">F54*0.000001</f>
+        <f t="shared" ref="P12:P22" si="0">F54*0.000001</f>
         <v>1.8924E-2</v>
       </c>
       <c r="Q12">
-        <f t="shared" ref="Q12:Q22" si="2">G54*0.000001</f>
+        <f t="shared" ref="Q12:Q22" si="1">G54*0.000001</f>
         <v>4.2651000000000001E-2</v>
       </c>
       <c r="R12">
-        <f t="shared" ref="R12:R22" si="3">H54*0.000001</f>
+        <f t="shared" ref="R12:R22" si="2">H54*0.000001</f>
         <v>1.1644E-2</v>
       </c>
       <c r="S12">
-        <f t="shared" ref="S12:S22" si="4">J32*0.000001</f>
-        <v>9.3793492999999994</v>
+        <f>J30*0.000001</f>
+        <v>6.0361E-3</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T12:T22" si="5">J2*0.000001</f>
+        <f>J2*0.000001</f>
         <v>7.0124999999999996E-3</v>
       </c>
       <c r="U12">
-        <f t="shared" ref="U12:U22" si="6">J17*0.000001</f>
-        <v>0.24125079999999999</v>
+        <f>J16*0.000001</f>
+        <v>6.3425E-3</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="D13">
-        <v>5990</v>
+        <v>1085945</v>
       </c>
       <c r="E13">
-        <v>65536</v>
+        <v>16777216</v>
       </c>
       <c r="F13">
-        <v>260460</v>
+        <v>100951137</v>
       </c>
       <c r="G13">
-        <v>151243</v>
+        <v>47769039</v>
       </c>
       <c r="H13">
-        <v>34514</v>
+        <v>8881538</v>
       </c>
       <c r="I13">
-        <v>11903</v>
+        <v>25573833</v>
       </c>
       <c r="J13">
         <f>SUM(F13:I13)/10</f>
-        <v>45812</v>
+        <v>18317554.699999999</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
-        <v>4.5811999999999999E-2</v>
+        <f>J13*0.000001</f>
+        <v>18.317554699999999</v>
       </c>
       <c r="L13" t="s">
         <v>161</v>
@@ -48318,28 +48307,28 @@
         <v>1.24935102462768</v>
       </c>
       <c r="P13">
+        <f t="shared" si="0"/>
+        <v>3.5549999999999998E-2</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="1"/>
-        <v>3.5549999999999998E-2</v>
-      </c>
-      <c r="Q13">
+        <v>7.2294999999999998E-2</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="2"/>
-        <v>7.2294999999999998E-2</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="3"/>
         <v>2.2445E-2</v>
       </c>
       <c r="S13">
-        <f t="shared" si="4"/>
-        <v>8.996541800000001</v>
+        <f t="shared" ref="S13:S26" si="3">J31*0.000001</f>
+        <v>1.20792E-2</v>
       </c>
       <c r="T13">
-        <f t="shared" si="5"/>
-        <v>6.3425E-3</v>
+        <f t="shared" ref="T12:T22" si="4">J3*0.000001</f>
+        <v>1.3460700000000001E-2</v>
       </c>
       <c r="U13">
-        <f t="shared" si="6"/>
-        <v>0.20122989999999999</v>
+        <f t="shared" ref="U13:U26" si="5">J17*0.000001</f>
+        <v>1.2343E-2</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -48347,36 +48336,36 @@
         <v>188</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="D14">
-        <v>11545</v>
+        <v>2105215</v>
       </c>
       <c r="E14">
-        <v>131072</v>
+        <v>33554432</v>
       </c>
       <c r="F14">
-        <v>538286</v>
+        <v>218385040</v>
       </c>
       <c r="G14">
-        <v>343296</v>
+        <v>103390137</v>
       </c>
       <c r="H14">
-        <v>79318</v>
+        <v>16997237</v>
       </c>
       <c r="I14">
-        <v>160466</v>
+        <v>56755334</v>
       </c>
       <c r="J14">
         <f>SUM(F14:I14)/10</f>
-        <v>112136.6</v>
+        <v>39552774.799999997</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
-        <v>0.1121366</v>
+        <f>J14*0.000001</f>
+        <v>39.552774799999995</v>
       </c>
       <c r="L14" t="s">
         <v>162</v>
@@ -48391,65 +48380,65 @@
         <v>2.4412760734558101</v>
       </c>
       <c r="P14">
+        <f t="shared" si="0"/>
+        <v>7.0655999999999997E-2</v>
+      </c>
+      <c r="Q14">
         <f t="shared" si="1"/>
-        <v>7.0655999999999997E-2</v>
-      </c>
-      <c r="Q14">
+        <v>9.1160999999999992E-2</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="2"/>
-        <v>9.1160999999999992E-2</v>
-      </c>
-      <c r="R14">
+        <v>4.8547E-2</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="3"/>
-        <v>4.8547E-2</v>
-      </c>
-      <c r="S14">
+        <v>2.6046900000000001E-2</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="4"/>
-        <v>8.2672998999999994</v>
-      </c>
-      <c r="T14">
+        <v>2.98672E-2</v>
+      </c>
+      <c r="U14">
         <f t="shared" si="5"/>
-        <v>6.0361E-3</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="6"/>
-        <v>0.19837249999999998</v>
+        <v>2.5030099999999996E-2</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="D15">
-        <v>11545</v>
+        <v>3996018</v>
       </c>
       <c r="E15">
-        <v>131072</v>
+        <v>67108864</v>
       </c>
       <c r="F15">
-        <v>537457</v>
+        <v>471162011</v>
       </c>
       <c r="G15">
-        <v>338904</v>
+        <v>209712716</v>
       </c>
       <c r="H15">
-        <v>76606</v>
+        <v>33517218</v>
       </c>
       <c r="I15">
-        <v>42022</v>
+        <v>132717119</v>
       </c>
       <c r="J15">
         <f>SUM(F15:I15)/10</f>
-        <v>99498.9</v>
+        <v>84710906.400000006</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
-        <v>9.9498899999999987E-2</v>
+        <f>J15*0.000001</f>
+        <v>84.710906399999999</v>
       </c>
       <c r="L15" t="s">
         <v>163</v>
@@ -48464,65 +48453,65 @@
         <v>4.7990965843200604</v>
       </c>
       <c r="P15">
+        <f t="shared" si="0"/>
+        <v>0.14288999999999999</v>
+      </c>
+      <c r="Q15">
         <f t="shared" si="1"/>
-        <v>0.14288999999999999</v>
-      </c>
-      <c r="Q15">
+        <v>0.182338</v>
+      </c>
+      <c r="R15">
         <f t="shared" si="2"/>
-        <v>0.182338</v>
-      </c>
-      <c r="R15">
+        <v>0.12656000000000001</v>
+      </c>
+      <c r="S15">
         <f t="shared" si="3"/>
-        <v>0.12656000000000001</v>
-      </c>
-      <c r="S15">
+        <v>4.5811999999999999E-2</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="4"/>
-        <v>18.317554699999999</v>
-      </c>
-      <c r="T15">
+        <v>5.6315099999999993E-2</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="5"/>
-        <v>1.3460700000000001E-2</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="6"/>
-        <v>0.50261339999999999</v>
+        <v>4.7463499999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>198</v>
-      </c>
-      <c r="B16" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" t="s">
-        <v>327</v>
-      </c>
-      <c r="D16">
-        <v>11545</v>
-      </c>
-      <c r="E16">
-        <v>131072</v>
-      </c>
-      <c r="F16">
-        <v>528652</v>
-      </c>
-      <c r="G16">
-        <v>308422</v>
-      </c>
-      <c r="H16">
-        <v>75586</v>
-      </c>
-      <c r="I16">
-        <v>24074</v>
-      </c>
-      <c r="J16">
+      <c r="A16" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="D16" s="61">
+        <v>854</v>
+      </c>
+      <c r="E16" s="61">
+        <v>8192</v>
+      </c>
+      <c r="F16" s="61">
+        <v>36768</v>
+      </c>
+      <c r="G16" s="61">
+        <v>20012</v>
+      </c>
+      <c r="H16" s="61">
+        <v>4182</v>
+      </c>
+      <c r="I16" s="61">
+        <v>2463</v>
+      </c>
+      <c r="J16" s="61">
         <f>SUM(F16:I16)/10</f>
-        <v>93673.4</v>
+        <v>6342.5</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
-        <v>9.367339999999999E-2</v>
+        <f>J16*0.000001</f>
+        <v>6.3425E-3</v>
       </c>
       <c r="L16" t="s">
         <v>164</v>
@@ -48537,65 +48526,65 @@
         <v>9.8714144229888898</v>
       </c>
       <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0.29174499999999998</v>
+      </c>
+      <c r="Q16">
         <f t="shared" si="1"/>
-        <v>0.29174499999999998</v>
-      </c>
-      <c r="Q16">
+        <v>0.40138799999999997</v>
+      </c>
+      <c r="R16">
         <f t="shared" si="2"/>
-        <v>0.40138799999999997</v>
-      </c>
-      <c r="R16">
+        <v>0.20809</v>
+      </c>
+      <c r="S16">
         <f t="shared" si="3"/>
-        <v>0.20809</v>
-      </c>
-      <c r="S16">
+        <v>9.367339999999999E-2</v>
+      </c>
+      <c r="T16">
         <f t="shared" si="4"/>
-        <v>16.260277899999998</v>
-      </c>
-      <c r="T16">
+        <v>0.1121366</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="5"/>
+        <v>9.9498899999999987E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="D17" s="61">
+        <v>1628</v>
+      </c>
+      <c r="E17" s="61">
+        <v>16384</v>
+      </c>
+      <c r="F17" s="61">
+        <v>68258</v>
+      </c>
+      <c r="G17" s="61">
+        <v>40767</v>
+      </c>
+      <c r="H17" s="61">
+        <v>9274</v>
+      </c>
+      <c r="I17" s="61">
+        <v>5131</v>
+      </c>
+      <c r="J17" s="61">
+        <f>SUM(F17:I17)/10</f>
+        <v>12343</v>
+      </c>
+      <c r="K17">
+        <f>J17*0.000001</f>
         <v>1.2343E-2</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="6"/>
-        <v>0.41348299999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17" t="s">
-        <v>328</v>
-      </c>
-      <c r="D17">
-        <v>22128</v>
-      </c>
-      <c r="E17">
-        <v>262144</v>
-      </c>
-      <c r="F17">
-        <v>1157352</v>
-      </c>
-      <c r="G17">
-        <v>725762</v>
-      </c>
-      <c r="H17">
-        <v>156026</v>
-      </c>
-      <c r="I17">
-        <v>373368</v>
-      </c>
-      <c r="J17">
-        <f>SUM(F17:I17)/10</f>
-        <v>241250.8</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>0.24125079999999999</v>
       </c>
       <c r="L17" t="s">
         <v>165</v>
@@ -48610,65 +48599,65 @@
         <v>21.5272326469421</v>
       </c>
       <c r="P17">
+        <f t="shared" si="0"/>
+        <v>0.59611099999999995</v>
+      </c>
+      <c r="Q17">
         <f t="shared" si="1"/>
-        <v>0.59611099999999995</v>
-      </c>
-      <c r="Q17">
+        <v>0.84992299999999998</v>
+      </c>
+      <c r="R17">
         <f t="shared" si="2"/>
-        <v>0.84992299999999998</v>
-      </c>
-      <c r="R17">
+        <v>0.43543599999999999</v>
+      </c>
+      <c r="S17">
         <f t="shared" si="3"/>
-        <v>0.43543599999999999</v>
-      </c>
-      <c r="S17">
+        <v>0.19837249999999998</v>
+      </c>
+      <c r="T17">
         <f t="shared" si="4"/>
-        <v>15.264897999999999</v>
-      </c>
-      <c r="T17">
+        <v>0.24125079999999999</v>
+      </c>
+      <c r="U17">
         <f t="shared" si="5"/>
-        <v>1.20792E-2</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="6"/>
-        <v>0.41080449999999996</v>
+        <v>0.20122989999999999</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="B18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C18" t="s">
-        <v>328</v>
-      </c>
-      <c r="D18">
-        <v>22128</v>
-      </c>
-      <c r="E18">
-        <v>262144</v>
-      </c>
-      <c r="F18">
-        <v>1108587</v>
-      </c>
-      <c r="G18">
-        <v>669274</v>
-      </c>
-      <c r="H18">
-        <v>149008</v>
-      </c>
-      <c r="I18">
-        <v>85430</v>
-      </c>
-      <c r="J18">
+      <c r="B18" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="D18" s="61">
+        <v>3115</v>
+      </c>
+      <c r="E18" s="61">
+        <v>32768</v>
+      </c>
+      <c r="F18" s="61">
+        <v>133543</v>
+      </c>
+      <c r="G18" s="61">
+        <v>89269</v>
+      </c>
+      <c r="H18" s="61">
+        <v>18697</v>
+      </c>
+      <c r="I18" s="61">
+        <v>8792</v>
+      </c>
+      <c r="J18" s="61">
         <f>SUM(F18:I18)/10</f>
-        <v>201229.9</v>
+        <v>25030.1</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
-        <v>0.20122989999999999</v>
+        <f>J18*0.000001</f>
+        <v>2.5030099999999996E-2</v>
       </c>
       <c r="L18" t="s">
         <v>166</v>
@@ -48683,65 +48672,65 @@
         <v>44.059046268463099</v>
       </c>
       <c r="P18">
+        <f t="shared" si="0"/>
+        <v>1.1876599999999999</v>
+      </c>
+      <c r="Q18">
         <f t="shared" si="1"/>
-        <v>1.1876599999999999</v>
-      </c>
-      <c r="Q18">
+        <v>1.703492</v>
+      </c>
+      <c r="R18">
         <f t="shared" si="2"/>
-        <v>1.703492</v>
-      </c>
-      <c r="R18">
+        <v>0.88026099999999996</v>
+      </c>
+      <c r="S18">
         <f t="shared" si="3"/>
-        <v>0.88026099999999996</v>
-      </c>
-      <c r="S18">
+        <v>0.41080449999999996</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="4"/>
-        <v>39.552774799999995</v>
-      </c>
-      <c r="T18">
+        <v>0.50261339999999999</v>
+      </c>
+      <c r="U18">
         <f t="shared" si="5"/>
-        <v>2.98672E-2</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="6"/>
-        <v>0.96447780000000005</v>
+        <v>0.41348299999999999</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>198</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" t="s">
-        <v>328</v>
-      </c>
-      <c r="D19">
-        <v>22128</v>
-      </c>
-      <c r="E19">
-        <v>262144</v>
-      </c>
-      <c r="F19">
-        <v>1104845</v>
-      </c>
-      <c r="G19">
-        <v>662889</v>
-      </c>
-      <c r="H19">
-        <v>149833</v>
-      </c>
-      <c r="I19">
-        <v>66158</v>
-      </c>
-      <c r="J19">
+      <c r="A19" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>326</v>
+      </c>
+      <c r="D19" s="61">
+        <v>5990</v>
+      </c>
+      <c r="E19" s="61">
+        <v>65536</v>
+      </c>
+      <c r="F19" s="61">
+        <v>262083</v>
+      </c>
+      <c r="G19" s="61">
+        <v>158521</v>
+      </c>
+      <c r="H19" s="61">
+        <v>36176</v>
+      </c>
+      <c r="I19" s="61">
+        <v>17855</v>
+      </c>
+      <c r="J19" s="61">
         <f>SUM(F19:I19)/10</f>
-        <v>198372.5</v>
+        <v>47463.5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
-        <v>0.19837249999999998</v>
+        <f>J19*0.000001</f>
+        <v>4.7463499999999999E-2</v>
       </c>
       <c r="L19" t="s">
         <v>167</v>
@@ -48756,65 +48745,65 @@
         <v>103.331104755401</v>
       </c>
       <c r="P19">
+        <f t="shared" si="0"/>
+        <v>2.3932729999999998</v>
+      </c>
+      <c r="Q19">
         <f t="shared" si="1"/>
-        <v>2.3932729999999998</v>
-      </c>
-      <c r="Q19">
+        <v>3.744024</v>
+      </c>
+      <c r="R19">
         <f t="shared" si="2"/>
-        <v>3.744024</v>
-      </c>
-      <c r="R19">
+        <v>1.9508829999999999</v>
+      </c>
+      <c r="S19">
         <f t="shared" si="3"/>
-        <v>1.9508829999999999</v>
-      </c>
-      <c r="S19">
+        <v>0.95031109999999996</v>
+      </c>
+      <c r="T19">
         <f t="shared" si="4"/>
-        <v>34.156629099999996</v>
-      </c>
-      <c r="T19">
+        <v>0.96447780000000005</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="5"/>
-        <v>2.5030099999999996E-2</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="6"/>
         <v>0.84638639999999998</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>188</v>
-      </c>
-      <c r="B20" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" t="s">
-        <v>329</v>
-      </c>
-      <c r="D20">
-        <v>42369</v>
-      </c>
-      <c r="E20">
-        <v>524288</v>
-      </c>
-      <c r="F20">
-        <v>2289625</v>
-      </c>
-      <c r="G20">
-        <v>1406313</v>
-      </c>
-      <c r="H20">
-        <v>318242</v>
-      </c>
-      <c r="I20">
-        <v>1011954</v>
-      </c>
-      <c r="J20">
+      <c r="A20" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="D20" s="61">
+        <v>11545</v>
+      </c>
+      <c r="E20" s="61">
+        <v>131072</v>
+      </c>
+      <c r="F20" s="61">
+        <v>537457</v>
+      </c>
+      <c r="G20" s="61">
+        <v>338904</v>
+      </c>
+      <c r="H20" s="61">
+        <v>76606</v>
+      </c>
+      <c r="I20" s="61">
+        <v>42022</v>
+      </c>
+      <c r="J20" s="61">
         <f>SUM(F20:I20)/10</f>
-        <v>502613.4</v>
+        <v>99498.9</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
-        <v>0.50261339999999999</v>
+        <f>J20*0.000001</f>
+        <v>9.9498899999999987E-2</v>
       </c>
       <c r="L20" t="s">
         <v>168</v>
@@ -48829,65 +48818,65 @@
         <v>198.93765258789</v>
       </c>
       <c r="P20">
+        <f t="shared" si="0"/>
+        <v>4.9277929999999994</v>
+      </c>
+      <c r="Q20">
         <f t="shared" si="1"/>
-        <v>4.9277929999999994</v>
-      </c>
-      <c r="Q20">
+        <v>8.1288719999999994</v>
+      </c>
+      <c r="R20">
         <f t="shared" si="2"/>
-        <v>8.1288719999999994</v>
-      </c>
-      <c r="R20">
+        <v>4.2727259999999996</v>
+      </c>
+      <c r="S20">
         <f t="shared" si="3"/>
-        <v>4.2727259999999996</v>
-      </c>
-      <c r="S20">
+        <v>1.7333896</v>
+      </c>
+      <c r="T20">
         <f t="shared" si="4"/>
-        <v>32.795722300000001</v>
-      </c>
-      <c r="T20">
+        <v>2.0467035</v>
+      </c>
+      <c r="U20">
         <f t="shared" si="5"/>
-        <v>2.6046900000000001E-2</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="6"/>
-        <v>0.95031109999999996</v>
+        <v>1.8156838</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="B21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" t="s">
-        <v>329</v>
-      </c>
-      <c r="D21">
-        <v>42369</v>
-      </c>
-      <c r="E21">
-        <v>524288</v>
-      </c>
-      <c r="F21">
-        <v>2363183</v>
-      </c>
-      <c r="G21">
-        <v>1329777</v>
-      </c>
-      <c r="H21">
-        <v>296183</v>
-      </c>
-      <c r="I21">
-        <v>145687</v>
-      </c>
-      <c r="J21">
+      <c r="B21" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>328</v>
+      </c>
+      <c r="D21" s="61">
+        <v>22128</v>
+      </c>
+      <c r="E21" s="61">
+        <v>262144</v>
+      </c>
+      <c r="F21" s="61">
+        <v>1108587</v>
+      </c>
+      <c r="G21" s="61">
+        <v>669274</v>
+      </c>
+      <c r="H21" s="61">
+        <v>149008</v>
+      </c>
+      <c r="I21" s="61">
+        <v>85430</v>
+      </c>
+      <c r="J21" s="61">
         <f>SUM(F21:I21)/10</f>
-        <v>413483</v>
+        <v>201229.9</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
-        <v>0.41348299999999999</v>
+        <f>J21*0.000001</f>
+        <v>0.20122989999999999</v>
       </c>
       <c r="L21" t="s">
         <v>169</v>
@@ -48902,448 +48891,440 @@
         <v>443.34885692596401</v>
       </c>
       <c r="P21">
+        <f t="shared" si="0"/>
+        <v>9.8902099999999997</v>
+      </c>
+      <c r="Q21">
         <f t="shared" si="1"/>
-        <v>9.8902099999999997</v>
-      </c>
-      <c r="Q21">
+        <v>17.788761999999998</v>
+      </c>
+      <c r="R21">
         <f t="shared" si="2"/>
-        <v>17.788761999999998</v>
-      </c>
-      <c r="R21">
+        <v>8.408631999999999</v>
+      </c>
+      <c r="S21">
         <f t="shared" si="3"/>
-        <v>8.408631999999999</v>
-      </c>
-      <c r="S21">
+        <v>3.7093542999999998</v>
+      </c>
+      <c r="T21">
         <f t="shared" si="4"/>
-        <v>84.710906399999999</v>
-      </c>
-      <c r="T21">
+        <v>4.3347607999999997</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="5"/>
-        <v>5.6315099999999993E-2</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="6"/>
-        <v>2.0467035</v>
+        <v>4.1810650000000003</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>198</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="61" t="s">
         <v>329</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="61">
         <v>42369</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="61">
         <v>524288</v>
       </c>
-      <c r="F22">
-        <v>2287993</v>
-      </c>
-      <c r="G22">
-        <v>1435821</v>
-      </c>
-      <c r="H22">
-        <v>284418</v>
-      </c>
-      <c r="I22">
-        <v>99813</v>
-      </c>
-      <c r="J22">
+      <c r="F22" s="61">
+        <v>2363183</v>
+      </c>
+      <c r="G22" s="61">
+        <v>1329777</v>
+      </c>
+      <c r="H22" s="61">
+        <v>296183</v>
+      </c>
+      <c r="I22" s="61">
+        <v>145687</v>
+      </c>
+      <c r="J22" s="61">
         <f>SUM(F22:I22)/10</f>
-        <v>410804.5</v>
+        <v>413483</v>
       </c>
       <c r="K22">
-        <f t="shared" si="0"/>
-        <v>0.41080449999999996</v>
+        <f>J22*0.000001</f>
+        <v>0.41348299999999999</v>
       </c>
       <c r="L22" t="s">
         <v>189</v>
       </c>
       <c r="P22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20.344567999999999</v>
       </c>
       <c r="Q22">
+        <f>G64*0.000001</f>
+        <v>41.733913000000001</v>
+      </c>
+      <c r="R22">
         <f t="shared" si="2"/>
-        <v>41.733913000000001</v>
-      </c>
-      <c r="R22">
+        <v>17.111107999999998</v>
+      </c>
+      <c r="S22">
         <f t="shared" si="3"/>
-        <v>17.111107999999998</v>
-      </c>
-      <c r="S22">
+        <v>8.2672998999999994</v>
+      </c>
+      <c r="T22">
         <f t="shared" si="4"/>
-        <v>70.832421699999998</v>
-      </c>
-      <c r="T22">
+        <v>9.3793492999999994</v>
+      </c>
+      <c r="U22">
         <f t="shared" si="5"/>
-        <v>4.7463499999999999E-2</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="6"/>
-        <v>1.8156838</v>
+        <v>8.996541800000001</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>188</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="61" t="s">
         <v>330</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="61">
         <v>81468</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="61">
         <v>1048576</v>
       </c>
-      <c r="F23">
-        <v>4720035</v>
-      </c>
-      <c r="G23">
-        <v>2942968</v>
-      </c>
-      <c r="H23">
-        <v>600752</v>
-      </c>
-      <c r="I23">
-        <v>1381023</v>
-      </c>
-      <c r="J23">
+      <c r="F23" s="61">
+        <v>4844206</v>
+      </c>
+      <c r="G23" s="61">
+        <v>2721676</v>
+      </c>
+      <c r="H23" s="61">
+        <v>570288</v>
+      </c>
+      <c r="I23" s="61">
+        <v>327694</v>
+      </c>
+      <c r="J23" s="61">
         <f>SUM(F23:I23)/10</f>
-        <v>964477.8</v>
+        <v>846386.4</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
-        <v>0.96447780000000005</v>
+        <f>J23*0.000001</f>
+        <v>0.84638639999999998</v>
       </c>
       <c r="L23" t="s">
         <v>190</v>
       </c>
       <c r="S23">
-        <f t="shared" ref="S23:S24" si="7">J43*0.000001</f>
-        <v>71.079053299999998</v>
+        <f t="shared" si="3"/>
+        <v>15.264897999999999</v>
       </c>
       <c r="T23">
-        <f t="shared" ref="T23:T26" si="8">J13*0.000001</f>
-        <v>4.5811999999999999E-2</v>
+        <f t="shared" ref="T23:T26" si="6">J13*0.000001</f>
+        <v>18.317554699999999</v>
       </c>
       <c r="U23">
-        <f t="shared" ref="U23:U26" si="9">J28*0.000001</f>
-        <v>1.7333896</v>
+        <f t="shared" si="5"/>
+        <v>16.260277899999998</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="B24" t="s">
-        <v>167</v>
-      </c>
-      <c r="C24" t="s">
-        <v>330</v>
-      </c>
-      <c r="D24">
-        <v>81468</v>
-      </c>
-      <c r="E24">
-        <v>1048576</v>
-      </c>
-      <c r="F24">
-        <v>4844206</v>
-      </c>
-      <c r="G24">
-        <v>2721676</v>
-      </c>
-      <c r="H24">
-        <v>570288</v>
-      </c>
-      <c r="I24">
-        <v>327694</v>
-      </c>
-      <c r="J24">
+      <c r="B24" s="61" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>331</v>
+      </c>
+      <c r="D24" s="61">
+        <v>155576</v>
+      </c>
+      <c r="E24" s="61">
+        <v>2097152</v>
+      </c>
+      <c r="F24" s="61">
+        <v>10728614</v>
+      </c>
+      <c r="G24" s="61">
+        <v>5638588</v>
+      </c>
+      <c r="H24" s="61">
+        <v>1175773</v>
+      </c>
+      <c r="I24" s="61">
+        <v>613863</v>
+      </c>
+      <c r="J24" s="61">
         <f>SUM(F24:I24)/10</f>
-        <v>846386.4</v>
+        <v>1815683.8</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
-        <v>0.84638639999999998</v>
+        <f>J24*0.000001</f>
+        <v>1.8156838</v>
       </c>
       <c r="L24" t="s">
         <v>191</v>
       </c>
       <c r="S24">
-        <f t="shared" si="7"/>
-        <v>147.71696619999997</v>
+        <f t="shared" si="3"/>
+        <v>32.795722300000001</v>
       </c>
       <c r="T24">
-        <f t="shared" si="8"/>
-        <v>0.1121366</v>
+        <f t="shared" si="6"/>
+        <v>39.552774799999995</v>
       </c>
       <c r="U24">
-        <f t="shared" si="9"/>
-        <v>4.3347607999999997</v>
+        <f t="shared" si="5"/>
+        <v>34.156629099999996</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C25" t="s">
-        <v>330</v>
-      </c>
-      <c r="D25">
-        <v>81468</v>
-      </c>
-      <c r="E25">
-        <v>1048576</v>
-      </c>
-      <c r="F25">
-        <v>4925602</v>
-      </c>
-      <c r="G25">
-        <v>3805431</v>
-      </c>
-      <c r="H25">
-        <v>580417</v>
-      </c>
-      <c r="I25">
-        <v>191661</v>
-      </c>
-      <c r="J25">
+      <c r="A25" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="61" t="s">
+        <v>332</v>
+      </c>
+      <c r="D25" s="61">
+        <v>296688</v>
+      </c>
+      <c r="E25" s="61">
+        <v>4194304</v>
+      </c>
+      <c r="F25" s="61">
+        <v>25644748</v>
+      </c>
+      <c r="G25" s="61">
+        <v>12585788</v>
+      </c>
+      <c r="H25" s="61">
+        <v>2217322</v>
+      </c>
+      <c r="I25" s="61">
+        <v>1362792</v>
+      </c>
+      <c r="J25" s="61">
         <f>SUM(F25:I25)/10</f>
-        <v>950311.1</v>
+        <v>4181065</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
-        <v>0.95031109999999996</v>
+        <f>J25*0.000001</f>
+        <v>4.1810650000000003</v>
       </c>
       <c r="L25" t="s">
         <v>192</v>
       </c>
       <c r="S25">
-        <f>J45*0.000001</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>71.079053299999998</v>
       </c>
       <c r="T25">
-        <f t="shared" si="8"/>
-        <v>9.9498899999999987E-2</v>
+        <f t="shared" si="6"/>
+        <v>84.710906399999999</v>
       </c>
       <c r="U25">
-        <f t="shared" si="9"/>
-        <v>4.1810650000000003</v>
+        <f t="shared" si="5"/>
+        <v>70.832421699999998</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>188</v>
-      </c>
-      <c r="B26" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" t="s">
-        <v>331</v>
-      </c>
-      <c r="D26">
-        <v>155576</v>
-      </c>
-      <c r="E26">
-        <v>2097152</v>
-      </c>
-      <c r="F26">
-        <v>10869235</v>
-      </c>
-      <c r="G26">
-        <v>5625590</v>
-      </c>
-      <c r="H26">
-        <v>1192874</v>
-      </c>
-      <c r="I26">
-        <v>2779336</v>
-      </c>
-      <c r="J26">
+      <c r="A26" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>333</v>
+      </c>
+      <c r="D26" s="61">
+        <v>575281</v>
+      </c>
+      <c r="E26" s="61">
+        <v>8388608</v>
+      </c>
+      <c r="F26" s="61">
+        <v>54157162</v>
+      </c>
+      <c r="G26" s="61">
+        <v>27829723</v>
+      </c>
+      <c r="H26" s="61">
+        <v>4599559</v>
+      </c>
+      <c r="I26" s="61">
+        <v>3378974</v>
+      </c>
+      <c r="J26" s="61">
         <f>SUM(F26:I26)/10</f>
-        <v>2046703.5</v>
+        <v>8996541.8000000007</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
-        <v>2.0467035</v>
+        <f>J26*0.000001</f>
+        <v>8.996541800000001</v>
       </c>
       <c r="L26" t="s">
         <v>193</v>
       </c>
       <c r="S26">
-        <f>J46*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <f t="shared" si="8"/>
-        <v>9.367339999999999E-2</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="9"/>
-        <v>3.7093542999999998</v>
+        <f t="shared" si="3"/>
+        <v>147.71696619999997</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="B27" t="s">
-        <v>168</v>
-      </c>
-      <c r="C27" t="s">
-        <v>331</v>
-      </c>
-      <c r="D27">
-        <v>155576</v>
-      </c>
-      <c r="E27">
-        <v>2097152</v>
-      </c>
-      <c r="F27">
-        <v>10728614</v>
-      </c>
-      <c r="G27">
-        <v>5638588</v>
-      </c>
-      <c r="H27">
-        <v>1175773</v>
-      </c>
-      <c r="I27">
-        <v>613863</v>
-      </c>
-      <c r="J27">
+      <c r="B27" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>335</v>
+      </c>
+      <c r="D27" s="61">
+        <v>1085945</v>
+      </c>
+      <c r="E27" s="61">
+        <v>16777216</v>
+      </c>
+      <c r="F27" s="61">
+        <v>101143611</v>
+      </c>
+      <c r="G27" s="61">
+        <v>47255336</v>
+      </c>
+      <c r="H27" s="61">
+        <v>8609911</v>
+      </c>
+      <c r="I27" s="61">
+        <v>5593921</v>
+      </c>
+      <c r="J27" s="61">
         <f>SUM(F27:I27)/10</f>
-        <v>1815683.8</v>
+        <v>16260277.9</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
-        <v>1.8156838</v>
+        <f>J27*0.000001</f>
+        <v>16.260277899999998</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>198</v>
-      </c>
-      <c r="B28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C28" t="s">
-        <v>331</v>
-      </c>
-      <c r="D28">
-        <v>155576</v>
-      </c>
-      <c r="E28">
-        <v>2097152</v>
-      </c>
-      <c r="F28">
-        <v>10519030</v>
-      </c>
-      <c r="G28">
-        <v>5308999</v>
-      </c>
-      <c r="H28">
-        <v>1159569</v>
-      </c>
-      <c r="I28">
-        <v>346298</v>
-      </c>
-      <c r="J28">
+      <c r="A28" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>336</v>
+      </c>
+      <c r="D28" s="61">
+        <v>2105215</v>
+      </c>
+      <c r="E28" s="61">
+        <v>33554432</v>
+      </c>
+      <c r="F28" s="61">
+        <v>221317526</v>
+      </c>
+      <c r="G28" s="61">
+        <v>92525216</v>
+      </c>
+      <c r="H28" s="61">
+        <v>16866480</v>
+      </c>
+      <c r="I28" s="61">
+        <v>10857069</v>
+      </c>
+      <c r="J28" s="61">
         <f>SUM(F28:I28)/10</f>
-        <v>1733389.6</v>
+        <v>34156629.100000001</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
-        <v>1.7333896</v>
+        <f>J28*0.000001</f>
+        <v>34.156629099999996</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>188</v>
-      </c>
-      <c r="B29" t="s">
-        <v>169</v>
-      </c>
-      <c r="C29" t="s">
-        <v>332</v>
-      </c>
-      <c r="D29">
-        <v>296688</v>
-      </c>
-      <c r="E29">
-        <v>4194304</v>
-      </c>
-      <c r="F29">
-        <v>22938768</v>
-      </c>
-      <c r="G29">
-        <v>12492948</v>
-      </c>
-      <c r="H29">
-        <v>2289086</v>
-      </c>
-      <c r="I29">
-        <v>5626806</v>
-      </c>
-      <c r="J29">
+      <c r="A29" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="B29" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29" s="61">
+        <v>3996018</v>
+      </c>
+      <c r="E29" s="61">
+        <v>67108864</v>
+      </c>
+      <c r="F29" s="61">
+        <v>464139527</v>
+      </c>
+      <c r="G29" s="61">
+        <v>189629666</v>
+      </c>
+      <c r="H29" s="61">
+        <v>32828127</v>
+      </c>
+      <c r="I29" s="61">
+        <v>21726897</v>
+      </c>
+      <c r="J29" s="61">
         <f>SUM(F29:I29)/10</f>
-        <v>4334760.8</v>
+        <v>70832421.700000003</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
-        <v>4.3347607999999997</v>
+        <f>J29*0.000001</f>
+        <v>70.832421699999998</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" t="s">
-        <v>332</v>
+        <v>160</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="D30">
-        <v>296688</v>
+        <v>854</v>
       </c>
       <c r="E30">
-        <v>4194304</v>
-      </c>
-      <c r="F30">
-        <v>25644748</v>
+        <v>8192</v>
+      </c>
+      <c r="F30" s="31">
+        <v>35106</v>
       </c>
       <c r="G30">
-        <v>12585788</v>
+        <v>18933</v>
       </c>
       <c r="H30">
-        <v>2217322</v>
+        <v>4157</v>
       </c>
       <c r="I30">
-        <v>1362792</v>
+        <v>2165</v>
       </c>
       <c r="J30">
         <f>SUM(F30:I30)/10</f>
-        <v>4181065</v>
+        <v>6036.1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
-        <v>4.1810650000000003</v>
+        <f>J30*0.000001</f>
+        <v>6.0361E-3</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
@@ -49351,110 +49332,110 @@
         <v>198</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D31">
-        <v>296688</v>
+        <v>1628</v>
       </c>
       <c r="E31">
-        <v>4194304</v>
+        <v>16384</v>
       </c>
       <c r="F31">
-        <v>22983316</v>
+        <v>67869</v>
       </c>
       <c r="G31">
-        <v>11314219</v>
+        <v>39739</v>
       </c>
       <c r="H31">
-        <v>2211353</v>
+        <v>9486</v>
       </c>
       <c r="I31">
-        <v>584655</v>
+        <v>3698</v>
       </c>
       <c r="J31">
         <f>SUM(F31:I31)/10</f>
-        <v>3709354.3</v>
+        <v>12079.2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
-        <v>3.7093542999999998</v>
+        <f>J31*0.000001</f>
+        <v>1.20792E-2</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D32">
-        <v>575281</v>
+        <v>3115</v>
       </c>
       <c r="E32">
-        <v>8388608</v>
+        <v>32768</v>
       </c>
       <c r="F32">
-        <v>51632958</v>
+        <v>132636</v>
       </c>
       <c r="G32">
-        <v>24887442</v>
+        <v>103646</v>
       </c>
       <c r="H32">
-        <v>4527503</v>
+        <v>17914</v>
       </c>
       <c r="I32">
-        <v>12745590</v>
+        <v>6273</v>
       </c>
       <c r="J32">
         <f>SUM(F32:I32)/10</f>
-        <v>9379349.3000000007</v>
+        <v>26046.9</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
-        <v>9.3793492999999994</v>
+        <f>J32*0.000001</f>
+        <v>2.6046900000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D33">
-        <v>575281</v>
+        <v>5990</v>
       </c>
       <c r="E33">
-        <v>8388608</v>
+        <v>65536</v>
       </c>
       <c r="F33">
-        <v>54157162</v>
+        <v>260460</v>
       </c>
       <c r="G33">
-        <v>27829723</v>
+        <v>151243</v>
       </c>
       <c r="H33">
-        <v>4599559</v>
+        <v>34514</v>
       </c>
       <c r="I33">
-        <v>3378974</v>
+        <v>11903</v>
       </c>
       <c r="J33">
         <f>SUM(F33:I33)/10</f>
-        <v>8996541.8000000007</v>
+        <v>45812</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
-        <v>8.996541800000001</v>
+        <f>J33*0.000001</f>
+        <v>4.5811999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
@@ -49462,110 +49443,110 @@
         <v>198</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="C34" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D34">
-        <v>575281</v>
+        <v>11545</v>
       </c>
       <c r="E34">
-        <v>8388608</v>
+        <v>131072</v>
       </c>
       <c r="F34">
-        <v>53664264</v>
+        <v>528652</v>
       </c>
       <c r="G34">
-        <v>23124422</v>
+        <v>308422</v>
       </c>
       <c r="H34">
-        <v>4455084</v>
+        <v>75586</v>
       </c>
       <c r="I34">
-        <v>1429229</v>
+        <v>24074</v>
       </c>
       <c r="J34">
         <f>SUM(F34:I34)/10</f>
-        <v>8267299.9000000004</v>
+        <v>93673.4</v>
       </c>
       <c r="K34">
-        <f t="shared" si="0"/>
-        <v>8.2672998999999994</v>
+        <f>J34*0.000001</f>
+        <v>9.367339999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B35" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="C35" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D35">
-        <v>1085945</v>
+        <v>22128</v>
       </c>
       <c r="E35">
-        <v>16777216</v>
+        <v>262144</v>
       </c>
       <c r="F35">
-        <v>100951137</v>
+        <v>1104845</v>
       </c>
       <c r="G35">
-        <v>47769039</v>
+        <v>662889</v>
       </c>
       <c r="H35">
-        <v>8881538</v>
+        <v>149833</v>
       </c>
       <c r="I35">
-        <v>25573833</v>
+        <v>66158</v>
       </c>
       <c r="J35">
         <f>SUM(F35:I35)/10</f>
-        <v>18317554.699999999</v>
+        <v>198372.5</v>
       </c>
       <c r="K35">
-        <f t="shared" si="0"/>
-        <v>18.317554699999999</v>
+        <f>J35*0.000001</f>
+        <v>0.19837249999999998</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D36">
-        <v>1085945</v>
+        <v>42369</v>
       </c>
       <c r="E36">
-        <v>16777216</v>
+        <v>524288</v>
       </c>
       <c r="F36">
-        <v>101143611</v>
+        <v>2287993</v>
       </c>
       <c r="G36">
-        <v>47255336</v>
+        <v>1435821</v>
       </c>
       <c r="H36">
-        <v>8609911</v>
+        <v>284418</v>
       </c>
       <c r="I36">
-        <v>5593921</v>
+        <v>99813</v>
       </c>
       <c r="J36">
         <f>SUM(F36:I36)/10</f>
-        <v>16260277.9</v>
+        <v>410804.5</v>
       </c>
       <c r="K36">
-        <f t="shared" si="0"/>
-        <v>16.260277899999998</v>
+        <f>J36*0.000001</f>
+        <v>0.41080449999999996</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="37" t="s">
@@ -49589,36 +49570,36 @@
         <v>198</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="C37" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D37">
-        <v>1085945</v>
+        <v>81468</v>
       </c>
       <c r="E37">
-        <v>16777216</v>
+        <v>1048576</v>
       </c>
       <c r="F37">
-        <v>102005381</v>
+        <v>4925602</v>
       </c>
       <c r="G37">
-        <v>40339236</v>
+        <v>3805431</v>
       </c>
       <c r="H37">
-        <v>8118158</v>
+        <v>580417</v>
       </c>
       <c r="I37">
-        <v>2186205</v>
+        <v>191661</v>
       </c>
       <c r="J37">
         <f>SUM(F37:I37)/10</f>
-        <v>15264898</v>
+        <v>950311.1</v>
       </c>
       <c r="K37">
-        <f t="shared" si="0"/>
-        <v>15.264897999999999</v>
+        <f>J37*0.000001</f>
+        <v>0.95031109999999996</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>154</v>
@@ -49653,154 +49634,154 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C38" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D38">
-        <v>2105215</v>
+        <v>155576</v>
       </c>
       <c r="E38">
-        <v>33554432</v>
+        <v>2097152</v>
       </c>
       <c r="F38">
-        <v>218385040</v>
+        <v>10519030</v>
       </c>
       <c r="G38">
-        <v>103390137</v>
+        <v>5308999</v>
       </c>
       <c r="H38">
-        <v>16997237</v>
+        <v>1159569</v>
       </c>
       <c r="I38">
-        <v>56755334</v>
+        <v>346298</v>
       </c>
       <c r="J38">
         <f>SUM(F38:I38)/10</f>
-        <v>39552774.799999997</v>
+        <v>1733389.6</v>
       </c>
       <c r="K38">
-        <f t="shared" si="0"/>
-        <v>39.552774799999995</v>
+        <f>J38*0.000001</f>
+        <v>1.7333896</v>
       </c>
       <c r="L38" t="s">
         <v>160</v>
       </c>
       <c r="M38">
-        <f t="shared" ref="M38:U38" si="10">ROUNDUP(M12,2)</f>
+        <f t="shared" ref="M38:U38" si="7">ROUNDUP(M12,2)</f>
         <v>0.7</v>
       </c>
       <c r="N38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.94000000000000006</v>
       </c>
       <c r="O38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.63</v>
       </c>
       <c r="P38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.05</v>
       </c>
       <c r="R38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
       <c r="S38">
-        <f t="shared" si="10"/>
-        <v>9.379999999999999</v>
+        <f t="shared" si="7"/>
+        <v>0.01</v>
       </c>
       <c r="T38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="U38">
-        <f t="shared" si="10"/>
-        <v>0.25</v>
+        <f t="shared" si="7"/>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="C39" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D39">
-        <v>2105215</v>
+        <v>296688</v>
       </c>
       <c r="E39">
-        <v>33554432</v>
+        <v>4194304</v>
       </c>
       <c r="F39">
-        <v>221317526</v>
+        <v>22983316</v>
       </c>
       <c r="G39">
-        <v>92525216</v>
+        <v>11314219</v>
       </c>
       <c r="H39">
-        <v>16866480</v>
+        <v>2211353</v>
       </c>
       <c r="I39">
-        <v>10857069</v>
+        <v>584655</v>
       </c>
       <c r="J39">
         <f>SUM(F39:I39)/10</f>
-        <v>34156629.100000001</v>
+        <v>3709354.3</v>
       </c>
       <c r="K39">
-        <f t="shared" si="0"/>
-        <v>34.156629099999996</v>
+        <f>J39*0.000001</f>
+        <v>3.7093542999999998</v>
       </c>
       <c r="L39" t="s">
         <v>161</v>
       </c>
       <c r="M39">
-        <f t="shared" ref="M39:U39" si="11">ROUNDUP(M13,2)</f>
+        <f t="shared" ref="M39:U39" si="8">ROUNDUP(M13,2)</f>
         <v>1.41</v>
       </c>
       <c r="N39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1.89</v>
       </c>
       <c r="O39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1.25</v>
       </c>
       <c r="P39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.04</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="R39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.03</v>
       </c>
       <c r="S39">
-        <f t="shared" si="11"/>
-        <v>9</v>
+        <f t="shared" si="8"/>
+        <v>0.02</v>
       </c>
       <c r="T39">
-        <f t="shared" si="11"/>
-        <v>0.01</v>
+        <f t="shared" si="8"/>
+        <v>0.02</v>
       </c>
       <c r="U39">
-        <f t="shared" si="11"/>
-        <v>0.21000000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.02</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
@@ -49808,227 +49789,227 @@
         <v>198</v>
       </c>
       <c r="B40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C40" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D40">
-        <v>2105215</v>
+        <v>575281</v>
       </c>
       <c r="E40">
-        <v>33554432</v>
+        <v>8388608</v>
       </c>
       <c r="F40">
-        <v>220039137</v>
+        <v>53664264</v>
       </c>
       <c r="G40">
-        <v>87235851</v>
+        <v>23124422</v>
       </c>
       <c r="H40">
-        <v>16496027</v>
+        <v>4455084</v>
       </c>
       <c r="I40">
-        <v>4186208</v>
+        <v>1429229</v>
       </c>
       <c r="J40">
         <f>SUM(F40:I40)/10</f>
-        <v>32795722.300000001</v>
+        <v>8267299.9000000004</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
-        <v>32.795722300000001</v>
+        <f>J40*0.000001</f>
+        <v>8.2672998999999994</v>
       </c>
       <c r="L40" t="s">
         <v>162</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40:U40" si="12">ROUNDUP(M14,2)</f>
+        <f t="shared" ref="M40:U40" si="9">ROUNDUP(M14,2)</f>
         <v>2.8</v>
       </c>
       <c r="N40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>3.78</v>
       </c>
       <c r="O40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>2.4499999999999997</v>
       </c>
       <c r="P40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.08</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="R40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="S40">
-        <f t="shared" si="12"/>
-        <v>8.27</v>
+        <f t="shared" si="9"/>
+        <v>0.03</v>
       </c>
       <c r="T40">
-        <f t="shared" si="12"/>
-        <v>0.01</v>
+        <f t="shared" si="9"/>
+        <v>0.03</v>
       </c>
       <c r="U40">
-        <f t="shared" si="12"/>
-        <v>0.2</v>
+        <f t="shared" si="9"/>
+        <v>0.03</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C41" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D41">
-        <v>3996018</v>
+        <v>1085945</v>
       </c>
       <c r="E41">
-        <v>67108864</v>
+        <v>16777216</v>
       </c>
       <c r="F41">
-        <v>471162011</v>
+        <v>102005381</v>
       </c>
       <c r="G41">
-        <v>209712716</v>
+        <v>40339236</v>
       </c>
       <c r="H41">
-        <v>33517218</v>
+        <v>8118158</v>
       </c>
       <c r="I41">
-        <v>132717119</v>
+        <v>2186205</v>
       </c>
       <c r="J41">
         <f>SUM(F41:I41)/10</f>
-        <v>84710906.400000006</v>
+        <v>15264898</v>
       </c>
       <c r="K41">
-        <f t="shared" si="0"/>
-        <v>84.710906399999999</v>
+        <f>J41*0.000001</f>
+        <v>15.264897999999999</v>
       </c>
       <c r="L41" t="s">
         <v>163</v>
       </c>
       <c r="M41">
-        <f t="shared" ref="M41:U41" si="13">ROUNDUP(M15,2)</f>
+        <f t="shared" ref="M41:U41" si="10">ROUNDUP(M15,2)</f>
         <v>5.87</v>
       </c>
       <c r="N41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>7.7</v>
       </c>
       <c r="O41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>4.8</v>
       </c>
       <c r="P41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0.19</v>
       </c>
       <c r="R41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0.13</v>
       </c>
       <c r="S41">
-        <f t="shared" si="13"/>
-        <v>18.32</v>
+        <f t="shared" si="10"/>
+        <v>0.05</v>
       </c>
       <c r="T41">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
+        <f t="shared" si="10"/>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="U41">
-        <f t="shared" si="13"/>
-        <v>0.51</v>
+        <f t="shared" si="10"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C42" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D42">
-        <v>3996018</v>
+        <v>2105215</v>
       </c>
       <c r="E42">
-        <v>67108864</v>
+        <v>33554432</v>
       </c>
       <c r="F42">
-        <v>464139527</v>
+        <v>220039137</v>
       </c>
       <c r="G42">
-        <v>189629666</v>
+        <v>87235851</v>
       </c>
       <c r="H42">
-        <v>32828127</v>
+        <v>16496027</v>
       </c>
       <c r="I42">
-        <v>21726897</v>
+        <v>4186208</v>
       </c>
       <c r="J42">
         <f>SUM(F42:I42)/10</f>
-        <v>70832421.700000003</v>
+        <v>32795722.300000001</v>
       </c>
       <c r="K42">
-        <f t="shared" si="0"/>
-        <v>70.832421699999998</v>
+        <f>J42*0.000001</f>
+        <v>32.795722300000001</v>
       </c>
       <c r="L42" t="s">
         <v>164</v>
       </c>
       <c r="M42">
-        <f t="shared" ref="M42:U42" si="14">ROUNDUP(M16,2)</f>
+        <f t="shared" ref="M42:U42" si="11">ROUNDUP(M16,2)</f>
         <v>11.959999999999999</v>
       </c>
       <c r="N42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>16.23</v>
       </c>
       <c r="O42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>9.879999999999999</v>
       </c>
       <c r="P42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.3</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.41000000000000003</v>
       </c>
       <c r="R42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.21000000000000002</v>
       </c>
       <c r="S42">
-        <f t="shared" si="14"/>
-        <v>16.270000000000003</v>
+        <f t="shared" si="11"/>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="T42">
-        <f t="shared" si="14"/>
-        <v>0.02</v>
+        <f t="shared" si="11"/>
+        <v>0.12</v>
       </c>
       <c r="U42">
-        <f t="shared" si="14"/>
-        <v>0.42</v>
+        <f t="shared" si="11"/>
+        <v>9.9999999999999992E-2</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
@@ -50064,47 +50045,47 @@
         <v>71079053.299999997</v>
       </c>
       <c r="K43">
-        <f t="shared" si="0"/>
+        <f>J43*0.000001</f>
         <v>71.079053299999998</v>
       </c>
       <c r="L43" t="s">
         <v>165</v>
       </c>
       <c r="M43">
-        <f t="shared" ref="M43:U43" si="15">ROUNDUP(M17,2)</f>
+        <f t="shared" ref="M43:U43" si="12">ROUNDUP(M17,2)</f>
         <v>24.94</v>
       </c>
       <c r="N43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>33.229999999999997</v>
       </c>
       <c r="O43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>21.53</v>
       </c>
       <c r="P43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>0.85</v>
       </c>
       <c r="R43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
       <c r="S43">
-        <f t="shared" si="15"/>
-        <v>15.27</v>
+        <f t="shared" si="12"/>
+        <v>0.2</v>
       </c>
       <c r="T43">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
+        <f t="shared" si="12"/>
+        <v>0.25</v>
       </c>
       <c r="U43">
-        <f t="shared" si="15"/>
-        <v>0.42</v>
+        <f t="shared" si="12"/>
+        <v>0.21000000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
@@ -50140,47 +50121,47 @@
         <v>147716966.19999999</v>
       </c>
       <c r="K44">
-        <f t="shared" si="0"/>
+        <f>J44*0.000001</f>
         <v>147.71696619999997</v>
       </c>
       <c r="L44" t="s">
         <v>166</v>
       </c>
       <c r="M44">
-        <f t="shared" ref="M44:U44" si="16">ROUNDUP(M18,2)</f>
+        <f t="shared" ref="M44:U44" si="13">ROUNDUP(M18,2)</f>
         <v>50.699999999999996</v>
       </c>
       <c r="N44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>68.61</v>
       </c>
       <c r="O44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>44.059999999999995</v>
       </c>
       <c r="P44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1.19</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1.71</v>
       </c>
       <c r="R44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>0.89</v>
       </c>
       <c r="S44">
-        <f t="shared" si="16"/>
-        <v>39.559999999999995</v>
+        <f t="shared" si="13"/>
+        <v>0.42</v>
       </c>
       <c r="T44">
-        <f t="shared" si="16"/>
-        <v>0.03</v>
+        <f t="shared" si="13"/>
+        <v>0.51</v>
       </c>
       <c r="U44">
-        <f t="shared" si="16"/>
-        <v>0.97</v>
+        <f t="shared" si="13"/>
+        <v>0.42</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
@@ -50188,39 +50169,39 @@
         <v>167</v>
       </c>
       <c r="M45">
-        <f t="shared" ref="M45:U45" si="17">ROUNDUP(M19,2)</f>
+        <f t="shared" ref="M45:U45" si="14">ROUNDUP(M19,2)</f>
         <v>101.80000000000001</v>
       </c>
       <c r="N45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>143.01</v>
       </c>
       <c r="O45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>103.34</v>
       </c>
       <c r="P45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>2.4</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>3.75</v>
       </c>
       <c r="R45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>1.96</v>
       </c>
       <c r="S45">
-        <f t="shared" si="17"/>
-        <v>34.159999999999997</v>
+        <f t="shared" si="14"/>
+        <v>0.96</v>
       </c>
       <c r="T45">
-        <f t="shared" si="17"/>
-        <v>0.03</v>
+        <f t="shared" si="14"/>
+        <v>0.97</v>
       </c>
       <c r="U45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>0.85</v>
       </c>
     </row>
@@ -50229,40 +50210,40 @@
         <v>168</v>
       </c>
       <c r="M46">
-        <f t="shared" ref="M46:U46" si="18">ROUNDUP(M20,2)</f>
+        <f t="shared" ref="M46:U46" si="15">ROUNDUP(M20,2)</f>
         <v>212.03</v>
       </c>
       <c r="N46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>308.40999999999997</v>
       </c>
       <c r="O46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>198.94</v>
       </c>
       <c r="P46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>4.93</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>8.129999999999999</v>
       </c>
       <c r="R46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>4.2799999999999994</v>
       </c>
       <c r="S46">
-        <f t="shared" si="18"/>
-        <v>32.799999999999997</v>
+        <f t="shared" si="15"/>
+        <v>1.74</v>
       </c>
       <c r="T46">
-        <f t="shared" si="18"/>
-        <v>0.03</v>
+        <f t="shared" si="15"/>
+        <v>2.0499999999999998</v>
       </c>
       <c r="U46">
-        <f t="shared" si="18"/>
-        <v>0.96</v>
+        <f t="shared" si="15"/>
+        <v>1.82</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
@@ -50270,40 +50251,40 @@
         <v>169</v>
       </c>
       <c r="M47">
-        <f t="shared" ref="M47:U47" si="19">ROUNDUP(M21,2)</f>
+        <f t="shared" ref="M47:U47" si="16">ROUNDUP(M21,2)</f>
         <v>417.5</v>
       </c>
       <c r="N47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>655.21</v>
       </c>
       <c r="O47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>443.34999999999997</v>
       </c>
       <c r="P47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>9.9</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>17.790000000000003</v>
       </c>
       <c r="R47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>8.41</v>
       </c>
       <c r="S47">
-        <f t="shared" si="19"/>
-        <v>84.72</v>
+        <f t="shared" si="16"/>
+        <v>3.71</v>
       </c>
       <c r="T47">
-        <f t="shared" si="19"/>
-        <v>6.0000000000000005E-2</v>
+        <f t="shared" si="16"/>
+        <v>4.34</v>
       </c>
       <c r="U47">
-        <f t="shared" si="19"/>
-        <v>2.0499999999999998</v>
+        <f t="shared" si="16"/>
+        <v>4.1899999999999995</v>
       </c>
       <c r="Y47" s="1" t="s">
         <v>232</v>
@@ -50326,40 +50307,40 @@
         <v>189</v>
       </c>
       <c r="M48">
-        <f t="shared" ref="M48:U48" si="20">ROUNDUP(M22,2)</f>
+        <f t="shared" ref="M48:U48" si="17">ROUNDUP(M22,2)</f>
         <v>0</v>
       </c>
       <c r="N48">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O48">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P48">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>20.350000000000001</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>41.739999999999995</v>
       </c>
       <c r="R48">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>17.12</v>
       </c>
       <c r="S48">
-        <f t="shared" si="20"/>
-        <v>70.84</v>
+        <f t="shared" si="17"/>
+        <v>8.27</v>
       </c>
       <c r="T48">
-        <f t="shared" si="20"/>
-        <v>0.05</v>
+        <f t="shared" si="17"/>
+        <v>9.379999999999999</v>
       </c>
       <c r="U48">
-        <f t="shared" si="20"/>
-        <v>1.82</v>
+        <f t="shared" si="17"/>
+        <v>9</v>
       </c>
       <c r="X48" t="s">
         <v>188</v>
@@ -50380,11 +50361,11 @@
         <v>2779336</v>
       </c>
       <c r="AD48">
-        <f>SUM(Z48:AC48)/10</f>
+        <f t="shared" ref="AD48:AD65" si="18">SUM(Z48:AC48)/10</f>
         <v>2046703.5</v>
       </c>
       <c r="AE48">
-        <f t="shared" ref="AE48:AE65" si="21">AD48*0.000001</f>
+        <f t="shared" ref="AE48:AE65" si="19">AD48*0.000001</f>
         <v>2.0467035</v>
       </c>
     </row>
@@ -50393,16 +50374,16 @@
         <v>190</v>
       </c>
       <c r="S49">
-        <f t="shared" ref="S49:U52" si="22">ROUNDUP(S23,2)</f>
-        <v>71.08</v>
+        <f t="shared" ref="S49:U52" si="20">ROUNDUP(S23,2)</f>
+        <v>15.27</v>
       </c>
       <c r="T49">
-        <f t="shared" si="22"/>
-        <v>0.05</v>
+        <f t="shared" si="20"/>
+        <v>18.32</v>
       </c>
       <c r="U49">
-        <f t="shared" si="22"/>
-        <v>1.74</v>
+        <f t="shared" si="20"/>
+        <v>16.270000000000003</v>
       </c>
       <c r="X49" t="s">
         <v>197</v>
@@ -50423,11 +50404,11 @@
         <v>613863</v>
       </c>
       <c r="AD49">
-        <f>SUM(Z49:AC49)/10</f>
+        <f t="shared" si="18"/>
         <v>1815683.8</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>1.8156838</v>
       </c>
     </row>
@@ -50436,16 +50417,16 @@
         <v>191</v>
       </c>
       <c r="S50">
-        <f t="shared" si="22"/>
-        <v>147.72</v>
+        <f t="shared" si="20"/>
+        <v>32.799999999999997</v>
       </c>
       <c r="T50">
-        <f t="shared" si="22"/>
-        <v>0.12</v>
+        <f t="shared" si="20"/>
+        <v>39.559999999999995</v>
       </c>
       <c r="U50">
-        <f t="shared" si="22"/>
-        <v>4.34</v>
+        <f t="shared" si="20"/>
+        <v>34.159999999999997</v>
       </c>
       <c r="X50" t="s">
         <v>198</v>
@@ -50466,11 +50447,11 @@
         <v>346298</v>
       </c>
       <c r="AD50">
-        <f>SUM(Z50:AC50)/10</f>
+        <f t="shared" si="18"/>
         <v>1733389.6</v>
       </c>
       <c r="AE50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>1.7333896</v>
       </c>
     </row>
@@ -50479,16 +50460,16 @@
         <v>192</v>
       </c>
       <c r="S51">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f>ROUNDUP(S25,2)</f>
+        <v>71.08</v>
       </c>
       <c r="T51">
-        <f t="shared" si="22"/>
-        <v>9.9999999999999992E-2</v>
+        <f t="shared" si="20"/>
+        <v>84.72</v>
       </c>
       <c r="U51">
-        <f t="shared" si="22"/>
-        <v>4.1899999999999995</v>
+        <f t="shared" si="20"/>
+        <v>70.84</v>
       </c>
       <c r="X51" t="s">
         <v>188</v>
@@ -50509,11 +50490,11 @@
         <v>5626806</v>
       </c>
       <c r="AD51">
-        <f>SUM(Z51:AC51)/10</f>
+        <f t="shared" si="18"/>
         <v>4334760.8</v>
       </c>
       <c r="AE51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>4.3347607999999997</v>
       </c>
     </row>
@@ -50522,16 +50503,16 @@
         <v>193</v>
       </c>
       <c r="S52">
-        <f>ROUNDUP(S26,2)</f>
+        <f t="shared" ref="S52" si="21">ROUNDUP(S26,2)</f>
+        <v>147.72</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T52">
-        <f t="shared" si="22"/>
-        <v>9.9999999999999992E-2</v>
-      </c>
       <c r="U52">
-        <f t="shared" si="22"/>
-        <v>3.71</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="X52" t="s">
         <v>197</v>
@@ -50552,21 +50533,21 @@
         <v>1362792</v>
       </c>
       <c r="AD52">
-        <f>SUM(Z52:AC52)/10</f>
+        <f t="shared" si="18"/>
         <v>4181065</v>
       </c>
       <c r="AE52">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>4.1810650000000003</v>
       </c>
     </row>
     <row r="53" spans="5:31" x14ac:dyDescent="0.2">
-      <c r="E53" s="38" t="s">
+      <c r="E53" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
       <c r="X53" t="s">
         <v>198</v>
       </c>
@@ -50586,11 +50567,11 @@
         <v>584655</v>
       </c>
       <c r="AD53">
-        <f>SUM(Z53:AC53)/10</f>
+        <f t="shared" si="18"/>
         <v>3709354.3</v>
       </c>
       <c r="AE53">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>3.7093542999999998</v>
       </c>
     </row>
@@ -50626,11 +50607,11 @@
         <v>12745590</v>
       </c>
       <c r="AD54">
-        <f>SUM(Z54:AC54)/10</f>
+        <f t="shared" si="18"/>
         <v>9379349.3000000007</v>
       </c>
       <c r="AE54">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>9.3793492999999994</v>
       </c>
     </row>
@@ -50666,11 +50647,11 @@
         <v>3378974</v>
       </c>
       <c r="AD55">
-        <f>SUM(Z55:AC55)/10</f>
+        <f t="shared" si="18"/>
         <v>8996541.8000000007</v>
       </c>
       <c r="AE55">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>8.996541800000001</v>
       </c>
     </row>
@@ -50706,11 +50687,11 @@
         <v>1429229</v>
       </c>
       <c r="AD56">
-        <f>SUM(Z56:AC56)/10</f>
+        <f t="shared" si="18"/>
         <v>8267299.9000000004</v>
       </c>
       <c r="AE56">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>8.2672998999999994</v>
       </c>
     </row>
@@ -50746,11 +50727,11 @@
         <v>25573833</v>
       </c>
       <c r="AD57">
-        <f>SUM(Z57:AC57)/10</f>
+        <f t="shared" si="18"/>
         <v>18317554.699999999</v>
       </c>
       <c r="AE57">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>18.317554699999999</v>
       </c>
     </row>
@@ -50768,16 +50749,16 @@
         <v>208090</v>
       </c>
       <c r="L58" s="8"/>
-      <c r="M58" s="46" t="s">
+      <c r="M58" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="N58" s="46"/>
+      <c r="N58" s="45"/>
       <c r="O58" s="8"/>
-      <c r="P58" s="47" t="s">
+      <c r="P58" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="Q58" s="48"/>
-      <c r="R58" s="49"/>
+      <c r="Q58" s="47"/>
+      <c r="R58" s="48"/>
       <c r="S58" s="29" t="s">
         <v>226</v>
       </c>
@@ -50802,11 +50783,11 @@
         <v>5593921</v>
       </c>
       <c r="AD58">
-        <f>SUM(Z58:AC58)/10</f>
+        <f t="shared" si="18"/>
         <v>16260277.9</v>
       </c>
       <c r="AE58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>16.260277899999998</v>
       </c>
     </row>
@@ -50867,11 +50848,11 @@
         <v>2186205</v>
       </c>
       <c r="AD59">
-        <f>SUM(Z59:AC59)/10</f>
+        <f t="shared" si="18"/>
         <v>15264898</v>
       </c>
       <c r="AE59">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>15.264897999999999</v>
       </c>
     </row>
@@ -50896,11 +50877,11 @@
       </c>
       <c r="N60" s="10">
         <f>S44</f>
-        <v>39.559999999999995</v>
+        <v>0.42</v>
       </c>
       <c r="O60" s="8">
         <f>ROUNDUP(M60/N60,2)</f>
-        <v>13252.99</v>
+        <v>1248304.77</v>
       </c>
       <c r="P60" s="4">
         <f>ROUNDUP(C69*0.000001,2)</f>
@@ -50938,11 +50919,11 @@
         <v>56755334</v>
       </c>
       <c r="AD60">
-        <f>SUM(Z60:AC60)/10</f>
+        <f t="shared" si="18"/>
         <v>39552774.799999997</v>
       </c>
       <c r="AE60">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>39.552774799999995</v>
       </c>
     </row>
@@ -50966,19 +50947,19 @@
         <v>1048576</v>
       </c>
       <c r="N61" s="10">
-        <f t="shared" ref="N61:N63" si="23">S45</f>
-        <v>34.159999999999997</v>
+        <f t="shared" ref="N61:N63" si="22">S45</f>
+        <v>0.96</v>
       </c>
       <c r="O61" s="8">
-        <f t="shared" ref="O61:O68" si="24">ROUNDUP(M61/N61,2)</f>
-        <v>30696.019999999997</v>
+        <f t="shared" ref="O61:O68" si="23">ROUNDUP(M61/N61,2)</f>
+        <v>1092266.67</v>
       </c>
       <c r="P61" s="4">
-        <f t="shared" ref="P61:P64" si="25">ROUNDUP(C70*0.000001,2)</f>
+        <f t="shared" ref="P61:P64" si="24">ROUNDUP(C70*0.000001,2)</f>
         <v>2.4</v>
       </c>
       <c r="Q61" s="12">
-        <f t="shared" ref="Q61:Q64" si="26">ROUNDUP((M61/P61),2)</f>
+        <f t="shared" ref="Q61:Q64" si="25">ROUNDUP((M61/P61),2)</f>
         <v>436906.67</v>
       </c>
       <c r="R61" s="4">
@@ -50986,7 +50967,7 @@
         <v>101.80000000000001</v>
       </c>
       <c r="S61" s="4">
-        <f t="shared" ref="S61:S63" si="27">ROUNDUP(M61/R61,2)</f>
+        <f t="shared" ref="S61:S63" si="26">ROUNDUP(M61/R61,2)</f>
         <v>10300.36</v>
       </c>
       <c r="T61" s="6"/>
@@ -51009,11 +50990,11 @@
         <v>10857069</v>
       </c>
       <c r="AD61">
-        <f>SUM(Z61:AC61)/10</f>
+        <f t="shared" si="18"/>
         <v>34156629.100000001</v>
       </c>
       <c r="AE61">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>34.156629099999996</v>
       </c>
     </row>
@@ -51037,19 +51018,19 @@
         <v>2097152</v>
       </c>
       <c r="N62" s="10">
+        <f t="shared" si="22"/>
+        <v>1.74</v>
+      </c>
+      <c r="O62" s="8">
         <f t="shared" si="23"/>
-        <v>32.799999999999997</v>
-      </c>
-      <c r="O62" s="8">
+        <v>1205259.78</v>
+      </c>
+      <c r="P62" s="4">
         <f t="shared" si="24"/>
-        <v>63937.57</v>
-      </c>
-      <c r="P62" s="4">
+        <v>4.93</v>
+      </c>
+      <c r="Q62" s="12">
         <f t="shared" si="25"/>
-        <v>4.93</v>
-      </c>
-      <c r="Q62" s="12">
-        <f t="shared" si="26"/>
         <v>425385.81</v>
       </c>
       <c r="R62" s="4">
@@ -51057,7 +51038,7 @@
         <v>212.03</v>
       </c>
       <c r="S62" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>9890.83</v>
       </c>
       <c r="T62" s="6"/>
@@ -51080,11 +51061,11 @@
         <v>4186208</v>
       </c>
       <c r="AD62">
-        <f>SUM(Z62:AC62)/10</f>
+        <f t="shared" si="18"/>
         <v>32795722.300000001</v>
       </c>
       <c r="AE62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>32.795722300000001</v>
       </c>
     </row>
@@ -51108,19 +51089,19 @@
         <v>4194304</v>
       </c>
       <c r="N63" s="10">
+        <f t="shared" si="22"/>
+        <v>3.71</v>
+      </c>
+      <c r="O63" s="8">
         <f t="shared" si="23"/>
-        <v>84.72</v>
-      </c>
-      <c r="O63" s="8">
+        <v>1130540.17</v>
+      </c>
+      <c r="P63" s="4">
         <f t="shared" si="24"/>
-        <v>49507.840000000004</v>
-      </c>
-      <c r="P63" s="4">
+        <v>9.9</v>
+      </c>
+      <c r="Q63" s="12">
         <f t="shared" si="25"/>
-        <v>9.9</v>
-      </c>
-      <c r="Q63" s="12">
-        <f t="shared" si="26"/>
         <v>423667.08</v>
       </c>
       <c r="R63" s="4">
@@ -51128,7 +51109,7 @@
         <v>417.5</v>
       </c>
       <c r="S63" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>10046.24</v>
       </c>
       <c r="T63" s="6"/>
@@ -51151,11 +51132,11 @@
         <v>132717119</v>
       </c>
       <c r="AD63">
-        <f>SUM(Z63:AC63)/10</f>
+        <f t="shared" si="18"/>
         <v>84710906.400000006</v>
       </c>
       <c r="AE63">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>84.710906399999999</v>
       </c>
     </row>
@@ -51180,18 +51161,18 @@
       </c>
       <c r="N64" s="10">
         <f>S48</f>
-        <v>70.84</v>
+        <v>8.27</v>
       </c>
       <c r="O64" s="8">
+        <f t="shared" si="23"/>
+        <v>126792.75</v>
+      </c>
+      <c r="P64" s="4">
         <f t="shared" si="24"/>
-        <v>14802.04</v>
-      </c>
-      <c r="P64" s="4">
-        <f t="shared" si="25"/>
         <v>20.350000000000001</v>
       </c>
       <c r="Q64" s="12">
-        <f t="shared" si="26"/>
+        <f>ROUNDUP((M64/P64),2)</f>
         <v>51527.08</v>
       </c>
       <c r="R64" s="36" t="s">
@@ -51220,11 +51201,11 @@
         <v>21726897</v>
       </c>
       <c r="AD64">
-        <f>SUM(Z64:AC64)/10</f>
+        <f t="shared" si="18"/>
         <v>70832421.700000003</v>
       </c>
       <c r="AE64">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>70.832421699999998</v>
       </c>
     </row>
@@ -51237,11 +51218,11 @@
       </c>
       <c r="N65" s="10">
         <f>S49</f>
-        <v>71.08</v>
+        <v>15.27</v>
       </c>
       <c r="O65" s="8">
-        <f t="shared" si="24"/>
-        <v>236032.87</v>
+        <f t="shared" si="23"/>
+        <v>1098704.3899999999</v>
       </c>
       <c r="P65" s="36" t="s">
         <v>313</v>
@@ -51275,11 +51256,11 @@
         <v>8841053</v>
       </c>
       <c r="AD65">
-        <f>SUM(Z65:AC65)/10</f>
+        <f t="shared" si="18"/>
         <v>71079053.299999997</v>
       </c>
       <c r="AE65">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>71.079053299999998</v>
       </c>
     </row>
@@ -51291,12 +51272,12 @@
         <v>33554432</v>
       </c>
       <c r="N66" s="10">
-        <f t="shared" ref="N66:N67" si="28">S50</f>
-        <v>147.72</v>
+        <f>S50</f>
+        <v>32.799999999999997</v>
       </c>
       <c r="O66" s="8">
-        <f t="shared" si="24"/>
-        <v>227148.88</v>
+        <f t="shared" si="23"/>
+        <v>1023000.98</v>
       </c>
       <c r="P66" s="36" t="s">
         <v>313</v>
@@ -51320,12 +51301,12 @@
         <v>67108864</v>
       </c>
       <c r="N67" s="10">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="O67" s="8" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <f t="shared" ref="N66:N67" si="27">S51</f>
+        <v>71.08</v>
+      </c>
+      <c r="O67" s="8">
+        <f>ROUNDUP(M67/N67,2)</f>
+        <v>944131.46</v>
       </c>
       <c r="P67" s="36" t="s">
         <v>313</v>
@@ -51350,11 +51331,11 @@
       </c>
       <c r="N68" s="10">
         <f>S52</f>
-        <v>0</v>
-      </c>
-      <c r="O68" s="8" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>147.72</v>
+      </c>
+      <c r="O68" s="8">
+        <f t="shared" si="23"/>
+        <v>908595.51</v>
       </c>
       <c r="P68" s="36" t="s">
         <v>313</v>
@@ -51377,14 +51358,14 @@
       <c r="N69" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="O69" s="11" t="e">
+      <c r="O69" s="11">
         <f>ROUNDUP(AVERAGE(O60:O68),2)</f>
-        <v>#DIV/0!</v>
+        <v>975288.5</v>
       </c>
       <c r="P69" s="4"/>
       <c r="Q69" s="11">
-        <f>AVERAGE(Q64:Q68)</f>
-        <v>51527.08</v>
+        <f>ROUNDUP(AVERAGE(Q60:Q64),0)</f>
+        <v>355613</v>
       </c>
       <c r="R69" s="4"/>
       <c r="S69" s="3">
@@ -51445,277 +51426,277 @@
     </row>
     <row r="76" spans="3:31" x14ac:dyDescent="0.2">
       <c r="F76">
-        <f>M38/P38</f>
+        <f>ROUNDUP(M38/P38,0)</f>
         <v>35</v>
       </c>
       <c r="G76">
-        <f>N38/Q38</f>
-        <v>18.8</v>
+        <f>ROUNDUP(N38/Q38,0)</f>
+        <v>19</v>
       </c>
       <c r="H76">
-        <f t="shared" ref="H76:H85" si="29">O38/R38</f>
-        <v>31.5</v>
+        <f>ROUNDUP(O38/R38,0)</f>
+        <v>32</v>
       </c>
       <c r="I76">
-        <f>M38/S38</f>
-        <v>7.4626865671641798E-2</v>
+        <f>ROUNDUP(M38/S38,0)</f>
+        <v>70</v>
       </c>
       <c r="J76">
-        <f t="shared" ref="J76:K85" si="30">N38/T38</f>
+        <f>ROUNDUP(N38/T38,0)</f>
         <v>94</v>
       </c>
       <c r="K76">
-        <f t="shared" si="30"/>
-        <v>2.52</v>
+        <f>ROUNDUP(O38/U38,0)</f>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="3:31" x14ac:dyDescent="0.2">
       <c r="F77">
-        <f t="shared" ref="F77:F82" si="31">M39/P39</f>
-        <v>35.25</v>
+        <f t="shared" ref="F77:F85" si="28">ROUNDUP(M39/P39,0)</f>
+        <v>36</v>
       </c>
       <c r="G77">
-        <f t="shared" ref="G77:G85" si="32">N39/Q39</f>
-        <v>23.625</v>
+        <f t="shared" ref="G77:G85" si="29">ROUNDUP(N39/Q39,0)</f>
+        <v>24</v>
       </c>
       <c r="H77">
-        <f t="shared" si="29"/>
-        <v>41.666666666666671</v>
+        <f t="shared" ref="H77:H85" si="30">ROUNDUP(O39/R39,0)</f>
+        <v>42</v>
       </c>
       <c r="I77">
-        <f t="shared" ref="I77:I85" si="33">M39/S39</f>
-        <v>0.15666666666666665</v>
+        <f t="shared" ref="I77:I85" si="31">ROUNDUP(M39/S39,0)</f>
+        <v>71</v>
       </c>
       <c r="J77">
-        <f t="shared" si="30"/>
-        <v>189</v>
+        <f t="shared" ref="J77:J85" si="32">ROUNDUP(N39/T39,0)</f>
+        <v>95</v>
       </c>
       <c r="K77">
-        <f t="shared" si="30"/>
-        <v>5.9523809523809517</v>
+        <f t="shared" ref="K77:K85" si="33">ROUNDUP(O39/U39,0)</f>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="3:31" x14ac:dyDescent="0.2">
       <c r="F78">
+        <f t="shared" si="28"/>
+        <v>35</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="29"/>
+        <v>38</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="30"/>
+        <v>49</v>
+      </c>
+      <c r="I78">
         <f t="shared" si="31"/>
-        <v>35</v>
-      </c>
-      <c r="G78">
+        <v>94</v>
+      </c>
+      <c r="J78">
         <f t="shared" si="32"/>
-        <v>37.800000000000004</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="29"/>
-        <v>48.999999999999993</v>
-      </c>
-      <c r="I78">
+        <v>126</v>
+      </c>
+      <c r="K78">
         <f t="shared" si="33"/>
-        <v>0.3385731559854897</v>
-      </c>
-      <c r="J78">
-        <f t="shared" si="30"/>
-        <v>378</v>
-      </c>
-      <c r="K78">
-        <f t="shared" si="30"/>
-        <v>12.249999999999998</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="3:31" x14ac:dyDescent="0.2">
       <c r="F79">
+        <f t="shared" si="28"/>
+        <v>40</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="29"/>
+        <v>41</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="30"/>
+        <v>37</v>
+      </c>
+      <c r="I79">
         <f t="shared" si="31"/>
-        <v>39.133333333333326</v>
-      </c>
-      <c r="G79">
+        <v>118</v>
+      </c>
+      <c r="J79">
         <f t="shared" si="32"/>
-        <v>40.526315789473685</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="29"/>
-        <v>36.92307692307692</v>
-      </c>
-      <c r="I79">
+        <v>129</v>
+      </c>
+      <c r="K79">
         <f t="shared" si="33"/>
-        <v>0.32041484716157204</v>
-      </c>
-      <c r="J79">
-        <f t="shared" si="30"/>
-        <v>385</v>
-      </c>
-      <c r="K79">
-        <f t="shared" si="30"/>
-        <v>9.4117647058823533</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="3:31" x14ac:dyDescent="0.2">
       <c r="F80">
+        <f t="shared" si="28"/>
+        <v>40</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="29"/>
+        <v>40</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="30"/>
+        <v>48</v>
+      </c>
+      <c r="I80">
         <f t="shared" si="31"/>
-        <v>39.866666666666667</v>
-      </c>
-      <c r="G80">
+        <v>120</v>
+      </c>
+      <c r="J80">
         <f t="shared" si="32"/>
-        <v>39.585365853658537</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="29"/>
-        <v>47.047619047619037</v>
-      </c>
-      <c r="I80">
+        <v>136</v>
+      </c>
+      <c r="K80">
         <f t="shared" si="33"/>
-        <v>0.73509526736324504</v>
-      </c>
-      <c r="J80">
-        <f t="shared" si="30"/>
-        <v>811.5</v>
-      </c>
-      <c r="K80">
-        <f t="shared" si="30"/>
-        <v>23.523809523809522</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F81">
+        <f t="shared" si="28"/>
+        <v>42</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="29"/>
+        <v>40</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="30"/>
+        <v>49</v>
+      </c>
+      <c r="I81">
         <f t="shared" si="31"/>
-        <v>41.56666666666667</v>
-      </c>
-      <c r="G81">
+        <v>125</v>
+      </c>
+      <c r="J81">
         <f t="shared" si="32"/>
-        <v>39.094117647058823</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="29"/>
-        <v>48.931818181818187</v>
-      </c>
-      <c r="I81">
+        <v>133</v>
+      </c>
+      <c r="K81">
         <f t="shared" si="33"/>
-        <v>1.633267845448592</v>
-      </c>
-      <c r="J81">
-        <f t="shared" si="30"/>
-        <v>1661.4999999999998</v>
-      </c>
-      <c r="K81">
-        <f t="shared" si="30"/>
-        <v>51.261904761904766</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F82">
+        <f t="shared" si="28"/>
+        <v>43</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="29"/>
+        <v>41</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="30"/>
+        <v>50</v>
+      </c>
+      <c r="I82">
         <f t="shared" si="31"/>
-        <v>42.605042016806721</v>
-      </c>
-      <c r="G82">
+        <v>121</v>
+      </c>
+      <c r="J82">
         <f t="shared" si="32"/>
-        <v>40.122807017543863</v>
-      </c>
-      <c r="H82">
-        <f t="shared" si="29"/>
-        <v>49.505617977528082</v>
-      </c>
-      <c r="I82">
+        <v>135</v>
+      </c>
+      <c r="K82">
         <f t="shared" si="33"/>
-        <v>1.28159757330637</v>
-      </c>
-      <c r="J82">
-        <f t="shared" si="30"/>
-        <v>2287</v>
-      </c>
-      <c r="K82">
-        <f t="shared" si="30"/>
-        <v>45.422680412371129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F83">
-        <f>M45/P45</f>
-        <v>42.416666666666671</v>
+        <f t="shared" si="28"/>
+        <v>43</v>
       </c>
       <c r="G83">
+        <f t="shared" si="29"/>
+        <v>39</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="30"/>
+        <v>53</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="31"/>
+        <v>107</v>
+      </c>
+      <c r="J83">
         <f t="shared" si="32"/>
-        <v>38.135999999999996</v>
-      </c>
-      <c r="H83">
-        <f t="shared" si="29"/>
-        <v>52.724489795918373</v>
-      </c>
-      <c r="I83">
+        <v>148</v>
+      </c>
+      <c r="K83">
         <f t="shared" si="33"/>
-        <v>2.980093676814989</v>
-      </c>
-      <c r="J83">
-        <f t="shared" si="30"/>
-        <v>4767</v>
-      </c>
-      <c r="K83">
-        <f t="shared" si="30"/>
-        <v>121.5764705882353</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F84">
-        <f t="shared" ref="F84" si="34">M46/P46</f>
-        <v>43.008113590263697</v>
+        <f t="shared" si="28"/>
+        <v>44</v>
       </c>
       <c r="G84">
+        <f t="shared" si="29"/>
+        <v>38</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="30"/>
+        <v>47</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="31"/>
+        <v>122</v>
+      </c>
+      <c r="J84">
         <f t="shared" si="32"/>
-        <v>37.934809348093481</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="29"/>
-        <v>46.481308411214961</v>
-      </c>
-      <c r="I84">
+        <v>151</v>
+      </c>
+      <c r="K84">
         <f t="shared" si="33"/>
-        <v>6.4643292682926834</v>
-      </c>
-      <c r="J84">
-        <f t="shared" si="30"/>
-        <v>10280.333333333332</v>
-      </c>
-      <c r="K84">
-        <f t="shared" si="30"/>
-        <v>207.22916666666669</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F85">
-        <f>M47/P47</f>
-        <v>42.171717171717169</v>
+        <f t="shared" si="28"/>
+        <v>43</v>
       </c>
       <c r="G85">
+        <f t="shared" si="29"/>
+        <v>37</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="30"/>
+        <v>53</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="31"/>
+        <v>113</v>
+      </c>
+      <c r="J85">
         <f t="shared" si="32"/>
-        <v>36.830241708825177</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="29"/>
-        <v>52.717003567181919</v>
-      </c>
-      <c r="I85">
+        <v>151</v>
+      </c>
+      <c r="K85">
         <f t="shared" si="33"/>
-        <v>4.9279981114258735</v>
-      </c>
-      <c r="J85">
-        <f t="shared" si="30"/>
-        <v>10920.166666666666</v>
-      </c>
-      <c r="K85">
-        <f t="shared" si="30"/>
-        <v>216.26829268292684</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F87">
         <f>AVERAGE(F76:H86)</f>
-        <v>40.165682134926634</v>
+        <v>40.6</v>
       </c>
       <c r="I87">
         <f>AVERAGE(I76:K85)</f>
-        <v>1082.9276377857439</v>
+        <v>110.26666666666667</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J46">
-    <sortCondition ref="B2:B46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K44">
+    <sortCondition ref="A2:A44"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="F74:H74"/>

</xml_diff>